<commit_message>
feat: replace WhatsApp Hub with Fleet Overview on dashboard
- Remove WhatsApp Hub section from dashboard
- Add Fleet Overview component (ContainerFleetStats) in its place
- Update dashboard layout to show Service Requests alongside Fleet Overview
- Maintain responsive grid layout for better space utilization
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,55 +43,37 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T04:24:25.927Z</t>
+    <t>2025-11-25T04:53:21.081Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bf683b13-7f3a-4e71-a6e0-f57a6515837c","EventDtm":"2025-11-25T04:24:13Z","AppDtm":"2025-11-25T04:24:25Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:24:13Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.678689,"GPSLongitude":78.720108,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.3,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Faulty"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:24:13Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":29.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":230,"PSucQ":"asProvided","TDis":78.8,"TDisQ":null,"FreqComp":null,"TSuc":13.5,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":640,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":3.81,"TEvapQ":null,"MCtrl3":"EmergencyShutdown","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":94.88,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":397,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"AlarmShutdown","TRtn1":4.88,"TRtn1Q":null,"TRtn2":4.7,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.2,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":803,"RCAlias":"F803","RCSeverity":"Severe","Active":true},{"OemAlarm":809,"RCAlias":"F809","RCSeverity":"Severe","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:26:37.517Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"910fe96e-1d50-4f21-abdc-b546e4802a10","EventDtm":"2025-11-25T04:26:18Z","AppDtm":"2025-11-25T04:26:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:26:18Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.516006,"GPSLongitude":82.981248,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:26:18Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":29.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":147.13,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.49,"AmpPhB":11.1,"AmpPhC":11.49,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.11,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":95.51,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.04,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.46,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.63,"TRtn1Q":null,"TRtn2":4.67,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":9.35,"PctSucVlvQ":null,"TSup1":3.6,"TSup1Q":null,"TSup2":3.67,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:26:44.559Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"22cc4fd6-cb5c-44d9-a045-38f26d90a143","EventDtm":"2025-11-25T04:26:23Z","AppDtm":"2025-11-25T04:26:43Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:26:23Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479535,"GPSLongitude":73.969669,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:26:23Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":28.14,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":145.17,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":11.06,"AmpPhB":10.17,"AmpPhC":11.06,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.94,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":87.44,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.96,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.54,"TRtn1Q":null,"TRtn2":5.57,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.68,"PctSucVlvQ":null,"TSup1":4.92,"TSup1Q":null,"TSup2":4.94,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:29:28.011Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"262469a4-76cf-4078-89fe-c52c89bc3eec","EventDtm":"2025-11-25T04:29:03Z","AppDtm":"2025-11-25T04:29:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:29:03Z","DeviceID":"JSGA623040314","GPSLockState":"UNLOCKED","GPSSatelliteCount":11,"GPSLastLock":31,"GPSLatitude":19.252905,"GPSLongitude":73.016486,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:29:03Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":22.28,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.45,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":131.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.64,"AmpPhB":10.9,"AmpPhC":10.64,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.91,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.04,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.41,"TRtn1Q":null,"TRtn2":5.54,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":5.19,"PctSucVlvQ":null,"TSup1":7.95,"TSup1Q":null,"TSup2":5.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:33:51.547Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d229c1c9-439d-41ae-9524-b7ef6e0a0299","EventDtm":"2025-11-25T04:33:33Z","AppDtm":"2025-11-25T04:33:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:33:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.805012,"GPSLongitude":77.662298,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:33:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.65,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":99.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.52,"AmpPhB":11.17,"AmpPhC":11.52,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.25,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.18,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.85,"TRtn1Q":null,"TRtn2":5.87,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.13,"PctSucVlvQ":null,"TSup1":4.95,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:34:26.724Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"86c3d17b-7cb5-4cba-8b9a-140d8c02ab48","EventDtm":"2025-11-25T04:34:10Z","AppDtm":"2025-11-25T04:34:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:34:10Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892065,"GPSLongitude":79.476167,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:34:10Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":29.37,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":191.92,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":10.12,"AmpPhB":9.93,"AmpPhC":10.12,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.2,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":399.65,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.9,"TRtn1Q":null,"TRtn2":17.86,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.13,"PctSucVlvQ":null,"TSup1":18.54,"TSup1Q":null,"TSup2":18.58,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:34:31.785Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"380ae07c-ee34-45eb-8146-25da45ec08df","EventDtm":"2025-11-25T04:34:09Z","AppDtm":"2025-11-25T04:34:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:34:09Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.657874,"GPSLongitude":83.101755,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":28.8,"BatteryVoltage":7.9,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:34:09Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":29.85,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":0.32,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":176.29,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04742313","AmpPhA":13.46,"AmpPhB":13.18,"AmpPhC":13.46,"PDis":194.79,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.78,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":396.07,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.31,"TRtn1Q":null,"TRtn2":20.32,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":27,"PctSucVlvQ":null,"TSup1":18.26,"TSup1Q":null,"TSup2":18.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:34:51.308Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"932422f4-d38d-4fb6-8286-ac7b147623ad","EventDtm":"2025-11-25T04:34:37Z","AppDtm":"2025-11-25T04:34:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:34:37Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804998,"GPSLongitude":77.66231,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:34:37Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":27.25,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":158.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.3,"AmpPhB":10.72,"AmpPhC":10.3,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.01,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.4,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.91,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.36,"TRtn1Q":null,"TRtn2":5.37,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.22,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9cbf6af0-76d3-43e5-bd6d-e4c6b08283b7","EventDtm":"2025-11-25T04:50:39Z","AppDtm":"2025-11-25T04:51:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:50:39Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":28.678724,"GPSLongitude":77.599637,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.9,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:50:39Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":19.82,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":62.3,"PSucQ":null,"TDis":43.34,"TDisQ":null,"FreqComp":null,"TSuc":17.57,"TSucQ":null,"MCond":0,"PCond":276.17,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04475864","AmpPhA":1.58,"AmpPhB":1.53,"AmpPhC":1.58,"PDis":84.55,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":17.64,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":69.55,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.81,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.21,"TRtn1Q":null,"TRtn2":17.21,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":20,"PctSucVlvQ":null,"TSup1":17.58,"TSup1Q":null,"TSup2":17.6,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T04:53:48.274Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"584a3c61-46c6-4a37-bdd5-b29c92b54789","EventDtm":"2025-11-25T04:53:30Z","AppDtm":"2025-11-25T04:53:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:53:30Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":12.804897,"GPSLongitude":77.662165,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:53:30Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.78,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":98.72,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.46,"AmpPhB":10.92,"AmpPhC":11.46,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.79,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.1,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.86,"TRtn1Q":null,"TRtn2":5.88,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.76,"PctSucVlvQ":null,"TSup1":5.1,"TSup1Q":null,"TSup2":5.05,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T04:55:20.042Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"936fa6b6-851d-4513-ba3d-056a77c0e455","EventDtm":"2025-11-25T04:55:02Z","AppDtm":"2025-11-25T04:55:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:55:02Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.538987,"GPSLongitude":78.17834,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":46,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:55:02Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":29.81,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":70,"PSucQ":"asProvided","TDis":80.8,"TDisQ":null,"FreqComp":null,"TSuc":-13.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":990,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":94.21,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.2,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T04:56:43.542Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c29c27ca-bc62-4aa6-a7e4-9fc140faaa7d","EventDtm":"2025-11-25T04:56:25Z","AppDtm":"2025-11-25T04:56:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:56:25Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":26.606155,"GPSLongitude":80.723748,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T04:57:18.149Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b805d92d-ac79-4cc0-a4af-de818c839db0","EventDtm":"2025-11-25T04:57:02Z","AppDtm":"2025-11-25T04:57:17Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:57:02Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.572218,"GPSLongitude":78.515077,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323415","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":32.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
   </si>
 </sst>
 </file>
@@ -480,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -691,102 +673,6 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
feat: remove test alert simulation from dashboard and alerts page
- Remove test alert simulation section from dashboard
- Remove test alert simulation section from alerts page
- Clean up unused imports and state variables
- Remove simulateAlert mutations and related logic
- Streamline UI by removing development/testing features
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,106 +43,43 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T04:40:33.978Z</t>
+    <t>2025-11-25T05:09:32.858Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"910fe96e-1d50-4f21-abdc-b546e4802a10","EventDtm":"2025-11-25T04:26:18Z","AppDtm":"2025-11-25T04:26:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:26:18Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.516006,"GPSLongitude":82.981248,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:26:18Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":29.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":147.13,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.49,"AmpPhB":11.1,"AmpPhC":11.49,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.11,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":95.51,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.04,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.46,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.63,"TRtn1Q":null,"TRtn2":4.67,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":9.35,"PctSucVlvQ":null,"TSup1":3.6,"TSup1Q":null,"TSup2":3.67,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:40:34.042Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"22cc4fd6-cb5c-44d9-a045-38f26d90a143","EventDtm":"2025-11-25T04:26:23Z","AppDtm":"2025-11-25T04:26:43Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:26:23Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479535,"GPSLongitude":73.969669,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:26:23Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":28.14,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":145.17,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":11.06,"AmpPhB":10.17,"AmpPhC":11.06,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.94,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":87.44,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.96,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.54,"TRtn1Q":null,"TRtn2":5.57,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.68,"PctSucVlvQ":null,"TSup1":4.92,"TSup1Q":null,"TSup2":4.94,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"262469a4-76cf-4078-89fe-c52c89bc3eec","EventDtm":"2025-11-25T04:29:03Z","AppDtm":"2025-11-25T04:29:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:29:03Z","DeviceID":"JSGA623040314","GPSLockState":"UNLOCKED","GPSSatelliteCount":11,"GPSLastLock":31,"GPSLatitude":19.252905,"GPSLongitude":73.016486,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:29:03Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":22.28,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.45,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":131.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.64,"AmpPhB":10.9,"AmpPhC":10.64,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.91,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.04,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.41,"TRtn1Q":null,"TRtn2":5.54,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":5.19,"PctSucVlvQ":null,"TSup1":7.95,"TSup1Q":null,"TSup2":5.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:40:34.058Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d229c1c9-439d-41ae-9524-b7ef6e0a0299","EventDtm":"2025-11-25T04:33:33Z","AppDtm":"2025-11-25T04:33:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:33:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.805012,"GPSLongitude":77.662298,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:33:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.65,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":99.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.52,"AmpPhB":11.17,"AmpPhC":11.52,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.25,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.18,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.85,"TRtn1Q":null,"TRtn2":5.87,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.13,"PctSucVlvQ":null,"TSup1":4.95,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:40:34.065Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"86c3d17b-7cb5-4cba-8b9a-140d8c02ab48","EventDtm":"2025-11-25T04:34:10Z","AppDtm":"2025-11-25T04:34:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:34:10Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892065,"GPSLongitude":79.476167,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:34:10Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":29.37,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":191.92,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":10.12,"AmpPhB":9.93,"AmpPhC":10.12,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.2,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":399.65,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.9,"TRtn1Q":null,"TRtn2":17.86,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.13,"PctSucVlvQ":null,"TSup1":18.54,"TSup1Q":null,"TSup2":18.58,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:40:34.183Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"380ae07c-ee34-45eb-8146-25da45ec08df","EventDtm":"2025-11-25T04:34:09Z","AppDtm":"2025-11-25T04:34:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:34:09Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.657874,"GPSLongitude":83.101755,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":28.8,"BatteryVoltage":7.9,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:34:09Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":29.85,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":0.32,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":176.29,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04742313","AmpPhA":13.46,"AmpPhB":13.18,"AmpPhC":13.46,"PDis":194.79,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.78,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":396.07,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.31,"TRtn1Q":null,"TRtn2":20.32,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":27,"PctSucVlvQ":null,"TSup1":18.26,"TSup1Q":null,"TSup2":18.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:40:34.189Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"932422f4-d38d-4fb6-8286-ac7b147623ad","EventDtm":"2025-11-25T04:34:37Z","AppDtm":"2025-11-25T04:34:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:34:37Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804998,"GPSLongitude":77.66231,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:34:37Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":27.25,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":158.94,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.3,"AmpPhB":10.72,"AmpPhC":10.3,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.01,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.4,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.91,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.36,"TRtn1Q":null,"TRtn2":5.37,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.22,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.02,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:40:34.194Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30dbb108-5a23-451d-a6e4-cd9ceacdbd0d","EventDtm":"2025-11-25T04:36:10Z","AppDtm":"2025-11-25T04:36:24Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:36:10Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":21.735782,"GPSLongitude":72.628866,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"236857089","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Faulty"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:36:10Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":25.49,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":119.72,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Shutdown","SnCtrl":"04502009","AmpPhA":0,"AmpPhB":0.01,"AmpPhC":0,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.05,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":91.33,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":442.22,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.39,"TRtn1Q":null,"TRtn2":15.34,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":21,"PctSucVlvQ":null,"TSup1":15.03,"TSup1Q":null,"TSup2":15.2,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":24,"RCAlias":"AL24","RCSeverity":"Severe","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:43:48.919Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4378d95d-5800-4a8d-9fc1-93836c5a872c","EventDtm":"2025-11-25T04:43:30Z","AppDtm":"2025-11-25T04:43:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:43:30Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804964,"GPSLongitude":77.662335,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:43:30Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":31.55,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":98.83,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.39,"AmpPhB":10.92,"AmpPhC":11.39,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.2,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.96,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.59,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:45:48.942Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3ae81e1c-cc5a-4673-9752-2ce5904c73bd","EventDtm":"2025-11-25T04:45:32Z","AppDtm":"2025-11-25T04:45:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:45:32Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.657959,"GPSLongitude":83.101849,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8.1,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:45:32Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":30.94,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":69.39,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":125.96,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.89,"AmpPhB":1.51,"AmpPhC":0.89,"PDis":125.94,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.78,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":408.15,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.58,"TRtn1Q":null,"TRtn2":20.64,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":17.61,"PctSucVlvQ":null,"TSup1":19.82,"TSup1Q":null,"TSup2":19.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:49:58.230Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e98f6732-2fb9-4852-8d3d-454daf844c5c","EventDtm":"2025-11-25T04:49:43Z","AppDtm":"2025-11-25T04:49:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:49:43Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.533207,"GPSLongitude":78.433412,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":32.1,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:49:43Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":25.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":78.5,"TDisQ":null,"FreqComp":null,"TSuc":-32.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":790,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.9,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":8.84,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T04:51:10.081Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9cbf6af0-76d3-43e5-bd6d-e4c6b08283b7","EventDtm":"2025-11-25T04:50:39Z","AppDtm":"2025-11-25T04:51:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T04:50:39Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":28.678724,"GPSLongitude":77.599637,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.9,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T04:50:39Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":19.82,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":62.3,"PSucQ":null,"TDis":43.34,"TDisQ":null,"FreqComp":null,"TSuc":17.57,"TSucQ":null,"MCond":0,"PCond":276.17,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04475864","AmpPhA":1.58,"AmpPhB":1.53,"AmpPhC":1.58,"PDis":84.55,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":17.64,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":69.55,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.81,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.21,"TRtn1Q":null,"TRtn2":17.21,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":20,"PctSucVlvQ":null,"TSup1":17.58,"TSup1Q":null,"TSup2":17.6,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:01:39.502Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"41eb63a1-14af-4295-9f05-8cc84c71d179","EventDtm":"2025-11-25T05:01:21Z","AppDtm":"2025-11-25T05:01:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:01:21Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":21.735673,"GPSLongitude":72.628769,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"240697447","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Faulty"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:01:21Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":29.12,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":6,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":107.59,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Shutdown","SnCtrl":"04502009","AmpPhA":0,"AmpPhB":0,"AmpPhC":0,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.5,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90.93,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":444.14,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":1.69,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.25,"TRtn1Q":null,"TRtn2":17.21,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":19.03,"PctSucVlvQ":null,"TSup1":16.69,"TSup1Q":null,"TSup2":16.76,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":24,"RCAlias":"AL24","RCSeverity":"Severe","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:01:52.240Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0fa23eec-1b22-4124-8b62-b24c2ca107c8","EventDtm":"2025-11-25T05:01:33Z","AppDtm":"2025-11-25T05:01:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:01:33Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.644498,"GPSLongitude":88.467969,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323862","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Standby"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:02:39.684Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c7176821-1009-4f63-8cbe-a9d7dcb8f609","EventDtm":"2025-11-25T05:02:24Z","AppDtm":"2025-11-25T05:02:38Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:02:24Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":16.824767,"GPSLongitude":78.131626,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:02:24Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":29.31,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":73.2,"TDisQ":null,"FreqComp":null,"TSuc":-24.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1000,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":10.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":402.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.19,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.67,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":17,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:03:54.404Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4219e967-0c17-45e0-8820-10f61750a0ae","EventDtm":"2025-11-25T05:03:36Z","AppDtm":"2025-11-25T05:03:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:03:36Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":12.804835,"GPSLongitude":77.662195,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:03:36Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.38,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":103.08,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.57,"AmpPhB":10.8,"AmpPhC":11.57,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.11,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.84,"TRtn1Q":null,"TRtn2":5.86,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.12,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:05:45.619Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3069296c-1c74-4b2c-b7f5-110235cc7097","EventDtm":"2025-11-25T05:05:31Z","AppDtm":"2025-11-25T05:05:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:05:31Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.679062,"GPSLongitude":78.720067,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:05:31Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":25.38,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.03,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":137.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.1,"AmpPhB":10.76,"AmpPhC":11.1,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.78,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.71,"TRtn1Q":null,"TRtn2":4.71,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.65,"PctSucVlvQ":null,"TSup1":3.92,"TSup1Q":null,"TSup2":3.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3069296c-1c74-4b2c-b7f5-110235cc7097","EventDtm":"2025-11-25T05:05:31Z","AppDtm":"2025-11-25T05:05:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:05:31Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.679062,"GPSLongitude":78.720067,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:05:31Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":25.38,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.03,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":137.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.1,"AmpPhB":10.76,"AmpPhC":11.1,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.78,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.71,"TRtn1Q":null,"TRtn2":4.71,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.65,"PctSucVlvQ":null,"TSup1":3.92,"TSup1Q":null,"TSup2":3.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:09:32.929Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3aa492ca-003a-4aa8-a1eb-24189d6ec752","EventDtm":"2025-11-25T06:49:58Z","AppDtm":"2025-11-25T05:08:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T06:49:58Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3699,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":34.3,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:09:33.467Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"726959ca-0b44-4f97-9723-125c5a379a9e","EventDtm":"2025-11-25T05:09:08Z","AppDtm":"2025-11-25T05:09:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:09:08Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.661547,"GPSLongitude":83.089111,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:09:08Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":46.2,"TDisQ":null,"FreqComp":null,"TSuc":-14,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1060,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":367.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":98.78,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:10:38.675Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"aecd3425-d975-4115-960d-d7fb04ad05bf","EventDtm":"2025-11-25T05:10:22Z","AppDtm":"2025-11-25T05:10:37Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:10:22Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678715,"GPSLongitude":77.59958,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":4.7,"BatteryVoltage":7.9,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:11:21.444Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30770747-3acc-4083-ae91-0ed242ad587d","EventDtm":"2025-11-25T05:11:08Z","AppDtm":"2025-11-25T05:11:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:08Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":4,"GPSLatitude":19.252921,"GPSLongitude":73.016577,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:11:28.473Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2b5837cc-f513-403f-b53a-83c0ced9ccc6","EventDtm":"2025-11-25T05:11:07Z","AppDtm":"2025-11-25T05:11:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:07Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":12,"GPSLatitude":17.547937,"GPSLongitude":78.380464,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
   </si>
 </sst>
 </file>
@@ -531,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -648,7 +585,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -675,12 +612,12 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -707,12 +644,12 @@
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -739,12 +676,12 @@
         <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -771,359 +708,7 @@
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: restore useMutation import for alerts page functionality
- Add back useMutation import that was accidentally removed
- Required for acknowledge, resolve, and dispatch alert mutations
- Fixes blank screen and JavaScript errors on alerts page
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="31">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,43 +43,67 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T05:09:32.858Z</t>
+    <t>2025-11-25T05:14:11.272Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3069296c-1c74-4b2c-b7f5-110235cc7097","EventDtm":"2025-11-25T05:05:31Z","AppDtm":"2025-11-25T05:05:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:05:31Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.679062,"GPSLongitude":78.720067,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:05:31Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":25.38,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.03,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":137.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.1,"AmpPhB":10.76,"AmpPhC":11.1,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.78,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.71,"TRtn1Q":null,"TRtn2":4.71,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.65,"PctSucVlvQ":null,"TSup1":3.92,"TSup1Q":null,"TSup2":3.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:09:32.929Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3aa492ca-003a-4aa8-a1eb-24189d6ec752","EventDtm":"2025-11-25T06:49:58Z","AppDtm":"2025-11-25T05:08:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T06:49:58Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3699,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":34.3,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:09:33.467Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"726959ca-0b44-4f97-9723-125c5a379a9e","EventDtm":"2025-11-25T05:09:08Z","AppDtm":"2025-11-25T05:09:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:09:08Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.661547,"GPSLongitude":83.089111,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:09:08Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":46.2,"TDisQ":null,"FreqComp":null,"TSuc":-14,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1060,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":367.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":98.78,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:10:38.675Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"aecd3425-d975-4115-960d-d7fb04ad05bf","EventDtm":"2025-11-25T05:10:22Z","AppDtm":"2025-11-25T05:10:37Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:10:22Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678715,"GPSLongitude":77.59958,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":4.7,"BatteryVoltage":7.9,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:11:21.444Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30770747-3acc-4083-ae91-0ed242ad587d","EventDtm":"2025-11-25T05:11:08Z","AppDtm":"2025-11-25T05:11:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:08Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":4,"GPSLatitude":19.252921,"GPSLongitude":73.016577,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:11:28.473Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2b5837cc-f513-403f-b53a-83c0ced9ccc6","EventDtm":"2025-11-25T05:11:07Z","AppDtm":"2025-11-25T05:11:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:07Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":12,"GPSLatitude":17.547937,"GPSLongitude":78.380464,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3aa492ca-003a-4aa8-a1eb-24189d6ec752","EventDtm":"2025-11-25T06:49:58Z","AppDtm":"2025-11-25T05:08:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T06:49:58Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3699,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":34.3,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.322Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"726959ca-0b44-4f97-9723-125c5a379a9e","EventDtm":"2025-11-25T05:09:08Z","AppDtm":"2025-11-25T05:09:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:09:08Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.661547,"GPSLongitude":83.089111,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:09:08Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":46.2,"TDisQ":null,"FreqComp":null,"TSuc":-14,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1060,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":367.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":98.78,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.329Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"aecd3425-d975-4115-960d-d7fb04ad05bf","EventDtm":"2025-11-25T05:10:22Z","AppDtm":"2025-11-25T05:10:37Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:10:22Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678715,"GPSLongitude":77.59958,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":4.7,"BatteryVoltage":7.9,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.338Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30770747-3acc-4083-ae91-0ed242ad587d","EventDtm":"2025-11-25T05:11:08Z","AppDtm":"2025-11-25T05:11:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:08Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":4,"GPSLatitude":19.252921,"GPSLongitude":73.016577,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.352Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2b5837cc-f513-403f-b53a-83c0ced9ccc6","EventDtm":"2025-11-25T05:11:07Z","AppDtm":"2025-11-25T05:11:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:07Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":12,"GPSLatitude":17.547937,"GPSLongitude":78.380464,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.365Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ed025364-a08b-41c1-936f-e5a3efb7e401","EventDtm":"2025-11-25T05:12:05Z","AppDtm":"2025-11-25T05:12:42Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:12:05Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":26.310615,"GPSLongitude":91.717618,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.6,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:12:05Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":23.19,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":300,"PSucQ":"asProvided","TDis":22.9,"TDisQ":null,"FreqComp":null,"TSuc":20.9,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":300,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":404.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":46.62,"TRtn1Q":null,"TRtn2":11.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":50,"PctSucVlvQ":null,"TSup1":11,"TSup1Q":null,"TSup2":10.8,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.370Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"55df62f7-09ae-4619-8cff-e36059733f52","EventDtm":"2025-11-25T05:13:03Z","AppDtm":"2025-11-25T05:13:22Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:13:03Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.537149,"GPSLongitude":78.175627,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":27.6,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:13:03Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":28.09,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":174.4,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":8.93,"AmpPhB":10.39,"AmpPhC":8.93,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.8,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":11.25,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":394.61,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.83,"TRtn1Q":null,"TRtn2":-17.87,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.2,"TSup1Q":null,"TSup2":-31.59,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:14:11.475Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e0ae646c-e282-4094-80ed-29300cf60aba","EventDtm":"2025-11-25T05:13:32Z","AppDtm":"2025-11-25T05:13:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:13:32Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":12.804881,"GPSLongitude":77.662177,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:13:32Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":101.88,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.25,"AmpPhB":10.76,"AmpPhC":11.25,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.62,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.8,"TRtn1Q":null,"TRtn2":5.81,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.71,"PctSucVlvQ":null,"TSup1":4.97,"TSup1Q":null,"TSup2":4.92,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:15:00.123Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6d975b75-d8a9-4d89-81fe-d051c2f61815","EventDtm":"2025-11-25T05:14:43Z","AppDtm":"2025-11-25T05:14:59Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:14:43Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.310582,"GPSLongitude":91.717582,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8.1,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:14:43Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":23.38,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":310,"PSucQ":"asProvided","TDis":22.9,"TDisQ":null,"FreqComp":null,"TSuc":21.1,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":300,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":50,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"PTIEmergencyStop1","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":397.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":46.38,"TRtn1Q":null,"TRtn2":10.6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":50.3,"PctSucVlvQ":null,"TSup1":9.88,"TSup1Q":null,"TSup2":9.8,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T05:16:10.940Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0f08d980-a463-47ed-821b-34277681d5a9","EventDtm":"2025-11-25T05:15:54Z","AppDtm":"2025-11-25T05:16:10Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:15:54Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":26.3106,"GPSLongitude":91.717571,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8.1,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:15:54Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":23.38,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":180,"PSucQ":"asProvided","TDis":22.9,"TDisQ":null,"FreqComp":null,"TSuc":18.2,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1090,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":100,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":399.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":11.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":95.43,"PctSucVlvQ":null,"TSup1":10.69,"TSup1Q":null,"TSup2":10.5,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
   </si>
 </sst>
 </file>
@@ -468,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -711,6 +735,134 @@
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
feat: remove orbcomm-data page from application
- Remove orbcomm-data.tsx page file
- Remove route definition from App.tsx
- Remove navigation item from sidebar
- Clean up all references to /orbcomm-data endpoint
- Remove unused import from App.tsx
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="145">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,487 +43,409 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T09:14:23.724Z</t>
+    <t>2025-11-25T10:17:31.400Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c955e84b-7ea3-4a67-9e93-61634e34a072","EventDtm":"2025-11-25T07:13:33Z","AppDtm":"2025-11-25T07:13:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:13:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.804929,"GPSLongitude":77.66219,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:13:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.99,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":110.86,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.29,"AmpPhB":10.96,"AmpPhC":11.29,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.3,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.85,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.09,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.88,"TRtn1Q":null,"TRtn2":5.89,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.44,"PctSucVlvQ":null,"TSup1":5.09,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.752Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1db08936-1a67-4442-91a7-a4c713adfd8f","EventDtm":"2025-11-25T07:11:01Z","AppDtm":"2025-11-25T07:14:05Z","Events":["DeviceIsStationary"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:11:01Z","DeviceID":"JSGA622180064","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":17.542864,"GPSLongitude":78.226282,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"244465686","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.4,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1041571","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.763Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"33e25fba-8ca4-4f52-9f25-cb0a8271601d","EventDtm":"2025-11-25T07:15:09Z","AppDtm":"2025-11-25T07:15:46Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:15:09Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.678729,"GPSLongitude":78.720176,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8.1,"DeviceTemp":59,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:15:09Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":42.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":360,"PSucQ":"asProvided","TDis":38.1,"TDisQ":null,"FreqComp":null,"TSuc":44.3,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":620,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":13.69,"TEvapQ":null,"MCtrl3":"NonControl","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":90.94,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":396,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":14.31,"TRtn1Q":null,"TRtn2":14.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":15.12,"TSup1Q":null,"TSup2":15.1,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.769Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5f70cb43-da9b-4ee8-8607-7c4c78a65609","EventDtm":"2025-11-25T07:17:14Z","AppDtm":"2025-11-25T07:17:31Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:17:14Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":17.547707,"GPSLongitude":78.38059,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.9,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.776Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bed41003-89c5-4a0f-b9d9-c06ad65a65d8","EventDtm":"2025-11-25T07:19:17Z","AppDtm":"2025-11-25T07:19:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:19:17Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":16.892057,"GPSLongitude":79.47623,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.1,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:19:17Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":29.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":81.7,"TDisQ":null,"FreqComp":null,"TSuc":-26.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":890,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":-1.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":397.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.89,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.886Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4924b18d-6001-48a5-b905-784c32027b98","EventDtm":"2025-11-25T07:19:23Z","AppDtm":"2025-11-25T07:19:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:19:23Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.678747,"GPSLongitude":78.720136,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8.1,"DeviceTemp":58,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:19:23Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":36.88,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":86.6,"TDisQ":null,"FreqComp":null,"TSuc":-13.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1120,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":195,"PctExpVlvQ":"OOR","TEvap":8.81,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":74.02,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":12.31,"TRtn1Q":null,"TRtn2":12.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":9.62,"TSup1Q":null,"TSup2":9.6,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.926Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"47360d92-c477-4b57-b8e1-30061ef7cfd2","EventDtm":"2025-11-25T07:19:59Z","AppDtm":"2025-11-25T07:20:17Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:19:59Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.533108,"GPSLongitude":78.433056,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Standby"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.933Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4f306517-d3fd-4170-9d6a-f89eaca2b90d","EventDtm":"2025-11-25T07:20:58Z","AppDtm":"2025-11-25T07:21:14Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:20:58Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.606136,"GPSLongitude":80.723564,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":5.9,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.937Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7fb6a248-46ca-48f9-acf9-9be600c2b643","EventDtm":"2025-11-25T07:21:00Z","AppDtm":"2025-11-25T07:21:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:21:00Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":16.891855,"GPSLongitude":79.475959,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:21:00Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":29.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":73.3,"TDisQ":null,"FreqComp":null,"TSuc":-25.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1020,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":400.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.88,"TRtn1Q":null,"TRtn2":36.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.940Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a0abe3af-d4a5-4001-a17c-e471d5616222","EventDtm":"2025-11-25T07:20:58Z","AppDtm":"2025-11-25T07:21:23Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:20:58Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.606136,"GPSLongitude":80.723564,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":5.9,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.949Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"807e4b72-b230-4320-bcb3-c6bbcb31ed71","EventDtm":"2025-11-25T07:21:29Z","AppDtm":"2025-11-25T07:21:42Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:21:29Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.516158,"GPSLongitude":82.962358,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.7,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:21:29Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":29.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":60,"PSucQ":"asProvided","TDis":83.1,"TDisQ":null,"FreqComp":null,"TSuc":-7.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":880,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":47,"PctExpVlvQ":null,"TEvap":22.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":388.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.8,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.59,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.952Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ffc9e6ad-492c-44f3-a2e6-11471de07486","EventDtm":"2025-11-25T07:20:56Z","AppDtm":"2025-11-25T07:23:01Z","Events":["DeviceIsMoving"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:20:56Z","DeviceID":"JSGA622340507","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":17.684756,"GPSLongitude":83.171689,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"25792","CID":"233012267","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.7,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6616969","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.954Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"34a62451-1296-45ad-9e61-729b7f4d2cc3","EventDtm":"2025-11-25T07:23:33Z","AppDtm":"2025-11-25T07:23:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:23:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804883,"GPSLongitude":77.662184,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:23:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.82,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":109.64,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.52,"AmpPhB":11.15,"AmpPhC":11.52,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.85,"TRtn1Q":null,"TRtn2":5.87,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.66,"PctSucVlvQ":null,"TSup1":4.95,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.960Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"98e3d278-358f-412b-acc1-eded1ea31554","EventDtm":"2025-11-25T07:23:43Z","AppDtm":"2025-11-25T07:24:00Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:23:43Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":28.36474,"GPSLongitude":75.581334,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-83","ExtPower":true,"ExtPowerVoltage":34.4,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:23:43Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":22,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":36,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":6.1,"AmpPhB":7,"AmpPhC":6.9,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":6.7,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.961Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8227c1bc-2559-4154-b32b-bbbac5e97674","EventDtm":"2025-11-25T07:26:01Z","AppDtm":"2025-11-25T07:26:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:26:01Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.51592,"GPSLongitude":82.981121,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:26:01Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":30.39,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":144.35,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":12.13,"AmpPhB":11.18,"AmpPhC":12.13,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.42,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":95.52,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.83,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.17,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.92,"TRtn1Q":null,"TRtn2":5.01,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":10.46,"PctSucVlvQ":null,"TSup1":3.82,"TSup1Q":null,"TSup2":3.92,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.963Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"331e5b68-71a6-42f3-8381-9ab23ca940c8","EventDtm":"2025-11-25T07:26:32Z","AppDtm":"2025-11-25T07:26:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:26:32Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":15.479439,"GPSLongitude":73.969714,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082161","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:26:32Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.36,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":157.9,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.77,"AmpPhB":10.02,"AmpPhC":10.77,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.91,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.84,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.09,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.14,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.54,"TRtn1Q":null,"TRtn2":5.57,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.26,"PctSucVlvQ":null,"TSup1":4.85,"TSup1Q":null,"TSup2":4.87,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.965Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30ff5642-74e2-465c-a4ad-de4f58301ce3","EventDtm":"2025-11-25T07:28:34Z","AppDtm":"2025-11-25T07:29:07Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:28:34Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":28.678791,"GPSLongitude":77.599787,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:28:34Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":22.6,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":59.38,"PSucQ":null,"TDis":26.57,"TDisQ":null,"FreqComp":null,"TSuc":20.25,"TSucQ":null,"MCond":0,"PCond":265.81,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04475864","AmpPhA":1.61,"AmpPhB":1.68,"AmpPhC":1.61,"PDis":96.33,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.77,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":68.55,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.35,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":21.39,"TRtn1Q":null,"TRtn2":21.4,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":20.01,"TSup1Q":null,"TSup2":19.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.966Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"931270e2-77af-43b1-88f8-5a433c5e7ea3","EventDtm":"2025-11-25T07:29:41Z","AppDtm":"2025-11-25T07:30:04Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:29:41Z","DeviceID":"JSGA623040314","GPSLockState":"UNLOCKED","GPSSatelliteCount":9,"GPSLastLock":27,"GPSLatitude":19.252887,"GPSLongitude":73.01647,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:29:41Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":29.08,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":145.1,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":11.33,"AmpPhB":11.56,"AmpPhC":11.33,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.84,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.87,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.04,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.32,"TRtn1Q":null,"TRtn2":5.46,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":3.37,"PctSucVlvQ":null,"TSup1":8,"TSup1Q":null,"TSup2":5.03,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.968Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"55b0c985-8499-4dd3-9822-19af2d6bd231","EventDtm":"2025-11-25T07:30:14Z","AppDtm":"2025-11-25T07:30:29Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:30:14Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":26.606097,"GPSLongitude":80.723884,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":7.7,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.972Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0177088e-e1de-4868-a46a-60f9a88cd32e","EventDtm":"2025-11-25T07:30:14Z","AppDtm":"2025-11-25T07:30:39Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:30:14Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":26.606097,"GPSLongitude":80.723884,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":false,"ExtPowerVoltage":7.7,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:23.977Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"56a1a879-a26e-4181-b160-a1330dc9b59c","EventDtm":"2025-11-25T07:33:35Z","AppDtm":"2025-11-25T07:33:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:33:35Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804862,"GPSLongitude":77.662269,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:33:35Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.24,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":105.56,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.36,"AmpPhB":10.77,"AmpPhC":11.36,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.55,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.77,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.091Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"64bb922e-a23a-49bc-b2bf-8e35a9eeb269","EventDtm":"2025-11-25T07:34:41Z","AppDtm":"2025-11-25T07:34:58Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:34:41Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.65771,"GPSLongitude":83.101797,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":7.9,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:34:41Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":31.57,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":65.18,"PSucQ":null,"TDis":-192.58,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":138.8,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.93,"AmpPhB":1.54,"AmpPhC":0.93,"PDis":152.77,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.76,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.51,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.44,"TRtn1Q":null,"TRtn2":20.47,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":17.07,"PctSucVlvQ":null,"TSup1":19.95,"TSup1Q":null,"TSup2":19.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.136Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"dec3f28e-b5cd-4543-8d52-f73d2860e6f9","EventDtm":"2025-11-25T07:34:44Z","AppDtm":"2025-11-25T07:34:58Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:34:44Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":16.892095,"GPSLongitude":79.476165,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:34:44Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":32.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":153.19,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":11.34,"AmpPhB":11.06,"AmpPhC":11.34,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.08,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.21,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":402.35,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.85,"TRtn1Q":null,"TRtn2":17.79,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.29,"PctSucVlvQ":null,"TSup1":18.51,"TSup1Q":null,"TSup2":18.54,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.138Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":24,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"00a6f8d3-1d6e-49c6-9373-0d8946caeffa","EventDtm":"2025-11-25T07:34:57Z","AppDtm":"2025-11-25T07:35:15Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:34:57Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.804982,"GPSLongitude":77.662251,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:34:57Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":29.04,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":156.65,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.31,"AmpPhB":10.65,"AmpPhC":10.31,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.06,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.43,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.93,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.39,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.9,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.139Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":25,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a4a82be9-854e-46c5-9ff1-7d5667236f6d","EventDtm":"2025-11-25T07:36:29Z","AppDtm":"2025-11-25T07:36:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:36:29Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.57219,"GPSLongitude":78.515174,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323414","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.8,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.141Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":26,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"682e8d1c-94e3-4531-8c9a-8bbd577f0c48","EventDtm":"2025-11-25T07:40:59Z","AppDtm":"2025-11-25T07:41:12Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:40:59Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":28.679004,"GPSLongitude":77.599809,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":false,"ExtPowerVoltage":22.4,"BatteryVoltage":7.9,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.143Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":27,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"15b2b239-ca77-4189-ab76-cdcc23fb7496","EventDtm":"2025-11-25T07:42:26Z","AppDtm":"2025-11-25T07:42:43Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:42:26Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.31061,"GPSLongitude":91.717558,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":false,"ExtPowerVoltage":6.7,"BatteryVoltage":8,"DeviceTemp":43,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.145Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":28,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0b6ce2c9-9025-49b7-aeb4-75e20fda0c90","EventDtm":"2025-11-25T07:43:33Z","AppDtm":"2025-11-25T07:43:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:43:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804932,"GPSLongitude":77.662235,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:43:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.31,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":104.98,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.58,"AmpPhB":10.81,"AmpPhC":11.58,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.43,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.09,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.86,"TRtn1Q":null,"TRtn2":5.88,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.12,"PctSucVlvQ":null,"TSup1":5.09,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.147Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":29,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3d11b068-1585-433f-bf6e-579d87ad67a8","EventDtm":"2025-11-25T07:43:57Z","AppDtm":"2025-11-25T07:44:12Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:43:57Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.310608,"GPSLongitude":91.717555,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8,"DeviceTemp":43,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:43:57Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":30.31,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":59.2,"TDisQ":null,"FreqComp":null,"TSuc":1.8,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":230,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":408.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":44.88,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":46.04,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.152Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":30,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"28516e7f-36aa-4ba1-b56a-2752803bd31c","EventDtm":"2025-11-25T07:45:02Z","AppDtm":"2025-11-25T07:45:17Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:45:02Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.606187,"GPSLongitude":80.723741,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.155Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":31,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"edf60e8a-31f5-4682-ba7e-54557a4da55f","EventDtm":"2025-11-25T07:45:04Z","AppDtm":"2025-11-25T07:45:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:45:04Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.657809,"GPSLongitude":83.101778,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":30.1,"BatteryVoltage":8.1,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:45:04Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":32.71,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":70.69,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":125.5,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.92,"AmpPhB":1.54,"AmpPhC":0.92,"PDis":125.66,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.96,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.06,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.8,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.71,"TRtn1Q":null,"TRtn2":20.77,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":16.15,"PctSucVlvQ":null,"TSup1":20.27,"TSup1Q":null,"TSup2":20.36,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.163Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":32,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"dd850a9a-ae28-4328-8b37-1e35d8b19cc7","EventDtm":"2025-11-25T07:46:45Z","AppDtm":"2025-11-25T07:47:00Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:46:45Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":26.310621,"GPSLongitude":91.71753,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.5,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.164Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":33,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"10b69fc9-df0a-42cd-929d-addf92160ec1","EventDtm":"2025-11-25T07:47:47Z","AppDtm":"2025-11-25T07:48:03Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:47:47Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":26.310632,"GPSLongitude":91.717541,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":45,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:47:47Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":31.38,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":170,"PSucQ":"asProvided","TDis":52.6,"TDisQ":null,"FreqComp":null,"TSuc":4.3,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1330,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":100,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":6.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":113.41,"PctSucVlvQ":null,"TSup1":5.69,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.166Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":34,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6a4c2f07-3938-4e38-b2b5-e78f7da99589","EventDtm":"2025-11-25T07:50:12Z","AppDtm":"2025-11-25T07:50:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:50:12Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.533177,"GPSLongitude":78.433435,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8,"DeviceTemp":47,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:50:12Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":31.88,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":180,"PSucQ":"asProvided","TDis":64.2,"TDisQ":null,"FreqComp":null,"TSuc":1.6,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":880,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":13.69,"TEvapQ":null,"MCtrl3":"Defrost","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":100,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":422.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Defrost","TRtn1":6.88,"TRtn1Q":null,"TRtn2":7,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.38,"TSup1Q":null,"TSup2":4.5,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.167Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":35,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a5e49896-0cf8-463c-8712-fd145f8019d6","EventDtm":"2025-11-25T07:53:33Z","AppDtm":"2025-11-25T07:53:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:53:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.805046,"GPSLongitude":77.662273,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:53:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":34.12,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":114.13,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.72,"AmpPhB":11.05,"AmpPhC":11.72,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.27,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.7,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.86,"TRtn1Q":null,"TRtn2":5.87,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.83,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.168Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":36,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f39a362e-3430-43e6-a272-5a278fd22142","EventDtm":"2025-11-25T07:55:10Z","AppDtm":"2025-11-25T07:55:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:55:10Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.53901,"GPSLongitude":78.1783,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":40,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T07:55:10Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":30.19,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":107.9,"TDisQ":null,"FreqComp":null,"TSuc":-32.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":980,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":409.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":93.29,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.169Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":37,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d4729f19-13a8-4ed9-83fe-a78d89ff4542","EventDtm":"2025-11-25T07:59:02Z","AppDtm":"2025-11-25T08:00:45Z","Events":["DeviceIsMoving"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T07:59:02Z","DeviceID":"JSGA622180064","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":17.542703,"GPSLongitude":78.2444,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232147211","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.4,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1041571","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.170Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":38,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1951de47-0dd0-43cb-8bcb-b8a0b6b866a0","EventDtm":"2025-11-25T08:01:12Z","AppDtm":"2025-11-25T08:01:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:01:12Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":21.73568,"GPSLongitude":72.629018,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":30.9,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:01:12Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":32.43,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":185.35,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.88,"AmpPhB":13.4,"AmpPhC":13.88,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.32,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90.19,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":434.33,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.6,"TRtn1Q":null,"TRtn2":15.55,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.08,"PctSucVlvQ":null,"TSup1":14.96,"TSup1Q":null,"TSup2":15.13,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.176Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":39,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"960d44d6-39b8-4121-bb74-608a097f1a7c","EventDtm":"2025-11-25T08:01:30Z","AppDtm":"2025-11-25T08:01:44Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:01:30Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.572381,"GPSLongitude":78.515031,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"230807317","RSSI":"-69","ExtPower":false,"ExtPowerVoltage":6.1,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.179Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":40,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d0877cda-27a8-45a1-830d-4710e90be1d9","EventDtm":"2025-11-25T08:01:47Z","AppDtm":"2025-11-25T08:02:02Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:01:47Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":26.644606,"GPSLongitude":88.467983,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8.1,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Standby"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.181Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":41,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"53464214-0448-4d0b-91ad-8c3c730d51c5","EventDtm":"2025-11-25T08:02:30Z","AppDtm":"2025-11-25T08:02:43Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:02:30Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.82486,"GPSLongitude":78.131562,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":45,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:02:30Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":33.19,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":74.8,"TDisQ":null,"FreqComp":null,"TSuc":-21.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1170,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":10.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.89,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.186Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":42,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fc056513-2ded-40c4-a533-7737f3c3282a","EventDtm":"2025-11-25T08:03:39Z","AppDtm":"2025-11-25T08:03:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:03:39Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.80499,"GPSLongitude":77.662308,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:03:39Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.8,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":110.32,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.59,"AmpPhB":11.26,"AmpPhC":11.59,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.23,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.68,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.83,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.83,"PctSucVlvQ":null,"TSup1":4.92,"TSup1Q":null,"TSup2":4.83,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.187Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":43,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"86250654-600d-49e2-a7b8-d6910e14a78c","EventDtm":"2025-11-25T08:05:49Z","AppDtm":"2025-11-25T08:06:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:05:49Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.679138,"GPSLongitude":78.720359,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:05:49Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":30.05,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.42,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.91,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.16,"AmpPhB":10.85,"AmpPhC":11.16,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.4,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.74,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":407.17,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.08,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.95,"TRtn1Q":null,"TRtn2":4.95,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.21,"PctSucVlvQ":null,"TSup1":3.92,"TSup1Q":null,"TSup2":3.94,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":44,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9193a254-8a97-4330-bdb6-81fc6fd504fb","EventDtm":"2025-11-25T09:49:42Z","AppDtm":"2025-11-25T08:08:12Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:49:42Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3878,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34.2,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.188Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":45,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"49809c9f-a1b9-4246-b7e7-a41f823a0731","EventDtm":"2025-11-25T08:09:09Z","AppDtm":"2025-11-25T08:09:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:09:09Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661653,"GPSLongitude":83.089143,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8,"DeviceTemp":40,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:09:09Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":32,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":60,"PSucQ":"asProvided","TDis":48.4,"TDisQ":null,"FreqComp":null,"TSuc":-11.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1130,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":368.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":103.35,"PctSucVlvQ":"OOR","TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":46,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ca0a775e-6851-4c2e-9b47-e941214a7a00","EventDtm":"2025-11-25T08:12:16Z","AppDtm":"2025-11-25T08:12:33Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:12:16Z","DeviceID":"JSGA623040302","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":9,"GPSLatitude":19.253005,"GPSLongitude":73.016545,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.189Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":47,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"907d45db-2953-4e68-8f86-f09347e6f83e","EventDtm":"2025-11-25T08:12:58Z","AppDtm":"2025-11-25T08:13:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:12:58Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":194,"GPSLatitude":17.547937,"GPSLongitude":78.380464,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.3,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":48,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9fbfd091-0726-4f39-9e42-81f244d42737","EventDtm":"2025-11-25T08:13:00Z","AppDtm":"2025-11-25T08:13:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:13:00Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.537283,"GPSLongitude":78.175546,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:13:00Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":29.06,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":161.87,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":9.61,"AmpPhB":10.99,"AmpPhC":9.61,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.36,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":9.86,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":405.76,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.06,"TRtn1Q":null,"TRtn2":-17.1,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-32.21,"TSup1Q":null,"TSup2":-31.54,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":49,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5b227fe8-88b2-4ace-a077-e6572ffd59c6","EventDtm":"2025-11-25T08:13:34Z","AppDtm":"2025-11-25T08:13:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:13:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.805009,"GPSLongitude":77.662311,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:13:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.53,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":104.49,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.48,"AmpPhB":10.95,"AmpPhC":11.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.53,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.07,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.82,"TRtn1Q":null,"TRtn2":5.84,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.22,"PctSucVlvQ":null,"TSup1":5.06,"TSup1Q":null,"TSup2":4.98,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.190Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":50,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3658b2a0-dde0-4283-917e-41d983e0e8ae","EventDtm":"2025-11-25T08:17:22Z","AppDtm":"2025-11-25T08:17:39Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:17:22Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.547735,"GPSLongitude":78.380552,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.6,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.199Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":51,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b2760f7b-50ab-4179-a26a-166a167d4cba","EventDtm":"2025-11-25T08:17:51Z","AppDtm":"2025-11-25T08:18:04Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:17:51Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.572293,"GPSLongitude":78.515029,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323415","RSSI":"-69","ExtPower":false,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.294Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":52,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c050b73c-9615-4fc7-81b9-9f854d4fcac1","EventDtm":"2025-11-25T08:19:20Z","AppDtm":"2025-11-25T08:19:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:19:20Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.892047,"GPSLongitude":79.476233,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:19:20Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":30.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":83.5,"TDisQ":null,"FreqComp":null,"TSuc":-26.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":-1,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":400.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.2,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.324Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":53,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8248de78-d4bb-4175-b8be-2d222f4a3eee","EventDtm":"2025-11-25T08:19:19Z","AppDtm":"2025-11-25T08:19:37Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:19:19Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":17.678758,"GPSLongitude":78.720149,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8.1,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:19:19Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":34.88,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":30,"PSucQ":"asProvided","TDis":93.6,"TDisQ":null,"FreqComp":null,"TSuc":6.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":970,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":4,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":87.01,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.69,"TRtn1Q":null,"TRtn2":5.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":15.24,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":54,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"acee4706-81c3-4d59-b981-f14be212c1d4","EventDtm":"2025-11-25T08:20:06Z","AppDtm":"2025-11-25T08:20:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:20:06Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533657,"GPSLongitude":78.433216,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.5,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Standby"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.325Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":55,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f50f5e37-ba6f-40bf-8838-9c394ef91756","EventDtm":"2025-11-25T08:21:01Z","AppDtm":"2025-11-25T08:21:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:21:01Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891885,"GPSLongitude":79.475936,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:21:01Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":31.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":20,"PSucQ":"asProvided","TDis":81,"TDisQ":null,"FreqComp":null,"TSuc":-20.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1130,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":15,"PctExpVlvQ":null,"TEvap":3.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":401.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":7.19,"TRtn1Q":null,"TRtn2":37,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":13.11,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":56,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"886462d3-e70d-419f-883b-8429a49860d1","EventDtm":"2025-11-25T08:21:35Z","AppDtm":"2025-11-25T08:21:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:21:35Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":17.516158,"GPSLongitude":82.962357,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957963","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.5,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:21:35Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":30.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":30,"PSucQ":"asProvided","TDis":90.5,"TDisQ":null,"FreqComp":null,"TSuc":-7.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":19,"PctExpVlvQ":null,"TEvap":21.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":386.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.8,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":23.31,"TSup1Q":null,"TSup2":23.2,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":57,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5591a652-3eba-4229-bfe6-ffc6af8c6118","EventDtm":"2025-11-25T08:23:32Z","AppDtm":"2025-11-25T08:23:48Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:23:32Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":17.678709,"GPSLongitude":78.720184,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8.1,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:23:32Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":34.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":230,"PSucQ":"asProvided","TDis":93.5,"TDisQ":null,"FreqComp":null,"TSuc":6.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":710,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":3.81,"TEvapQ":null,"MCtrl3":"PTIEmergencyStop1","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":87.01,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":396.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.62,"TRtn1Q":null,"TRtn2":5.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":14.63,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":107,"RCAlias":"E107","RCSeverity":"Severe","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.326Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":58,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"10977f97-e993-4f5b-8b78-6a0d013243a3","EventDtm":"2025-11-25T08:23:33Z","AppDtm":"2025-11-25T08:23:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:23:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804961,"GPSLongitude":77.662292,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:23:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":34.18,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":115.57,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.56,"AmpPhB":11.18,"AmpPhC":11.56,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.29,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.05,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.87,"TRtn1Q":null,"TRtn2":5.89,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.89,"PctSucVlvQ":null,"TSup1":5.05,"TSup1Q":null,"TSup2":4.97,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":59,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7901901e-fbf1-4a73-a4bc-4c9c660be712","EventDtm":"2025-11-25T08:23:51Z","AppDtm":"2025-11-25T08:24:07Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:23:51Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":28.36474,"GPSLongitude":75.581314,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-81","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:23:51Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":23,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":36,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":8.3,"AmpPhB":9.3,"AmpPhC":9.4,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17.1,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.3,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":6.6,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.348Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":60,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d8f46a70-8330-46d4-b03f-4bc2fc2f4123","EventDtm":"2025-11-25T08:25:56Z","AppDtm":"2025-11-25T08:26:13Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:25:56Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.516116,"GPSLongitude":82.981168,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:25:56Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":30.54,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":142.91,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.99,"AmpPhB":11.33,"AmpPhC":11.99,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":94.93,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.32,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.15,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.85,"TRtn1Q":null,"TRtn2":3.89,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":8.39,"PctSucVlvQ":null,"TSup1":2.86,"TSup1Q":null,"TSup2":2.9,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.352Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":61,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"94d83817-3158-4219-92c3-2a994a9b1c0b","EventDtm":"2025-11-25T08:26:37Z","AppDtm":"2025-11-25T08:26:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:26:37Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479505,"GPSLongitude":73.969699,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":28.7,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:26:37Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":31.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":157.87,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.62,"AmpPhB":9.82,"AmpPhC":10.62,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.03,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.65,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.84,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.68,"TRtn1Q":null,"TRtn2":5.69,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":5.74,"PctSucVlvQ":null,"TSup1":4.98,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.354Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":62,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"169eb422-a18d-48c7-a04e-6ca77eb51407","EventDtm":"2025-11-25T08:27:04Z","AppDtm":"2025-11-25T08:27:23Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:27:04Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":17.678751,"GPSLongitude":78.720187,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8.1,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:27:04Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":34,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":90,"PSucQ":"asProvided","TDis":53.4,"TDisQ":null,"FreqComp":null,"TSuc":17.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":930,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":474,"PctExpVlvQ":"OOR","TEvap":4.69,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":88.19,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.69,"TRtn1Q":null,"TRtn2":5.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.69,"TSup1Q":null,"TSup2":4.7,"TSup2Q":null,"AmpTotalDraw":1,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.355Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":63,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3f0b0f1f-0b5b-40dc-8bec-2da314610313","EventDtm":"2025-11-25T08:28:25Z","AppDtm":"2025-11-25T08:30:12Z","Events":["DeviceIsStationary"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:28:25Z","DeviceID":"JSGA622180064","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.542477,"GPSLongitude":78.244763,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"250794005","RSSI":"-53","ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.4,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1041571","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":64,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d0c96dc3-c045-4fb3-8384-d130ce873040","EventDtm":"2025-11-25T08:29:54Z","AppDtm":"2025-11-25T08:30:16Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:29:54Z","DeviceID":"JSGA623040314","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":30,"GPSLatitude":19.252977,"GPSLongitude":73.016543,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:29:54Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":23.63,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.23,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":152.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":11.24,"AmpPhB":11.45,"AmpPhC":11.24,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.85,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":406.72,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.37,"TRtn1Q":null,"TRtn2":5.49,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":4.65,"PctSucVlvQ":null,"TSup1":7.91,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.356Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":65,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"32b2b002-f665-4206-86c2-3cc611488879","EventDtm":"2025-11-25T08:33:33Z","AppDtm":"2025-11-25T08:33:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:33:33Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.804929,"GPSLongitude":77.662264,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904096","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:33:33Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.65,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":107.65,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.55,"AmpPhB":11.38,"AmpPhC":11.55,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.23,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.83,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.11,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.84,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.91,"PctSucVlvQ":null,"TSup1":4.89,"TSup1Q":null,"TSup2":4.8,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":66,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f68c9370-59fb-4409-ad6f-a865361d5a1b","EventDtm":"2025-11-25T08:34:46Z","AppDtm":"2025-11-25T08:35:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:34:46Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657838,"GPSLongitude":83.101741,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":7.9,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:34:46Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":30.16,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":0.49,"PSucQ":null,"TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":176.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04742313","AmpPhA":13.64,"AmpPhB":13.28,"AmpPhC":13.64,"PDis":193.55,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.51,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":402.21,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.06,"TRtn1Q":null,"TRtn2":20.06,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":27,"PctSucVlvQ":null,"TSup1":17.47,"TSup1Q":null,"TSup2":17.5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.361Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":67,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ac00b912-37ed-4c3f-bb76-416fd5e56967","EventDtm":"2025-11-25T08:34:55Z","AppDtm":"2025-11-25T08:35:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:34:55Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":22,"GPSLastLock":0,"GPSLatitude":16.89212,"GPSLongitude":79.476198,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:34:55Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":31.92,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-191.8,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":157.64,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Startup","SnCtrl":"04251422","AmpPhA":11.37,"AmpPhB":11.2,"AmpPhC":11.37,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.09,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.21,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":402.28,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.88,"TRtn1Q":null,"TRtn2":17.81,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.22,"PctSucVlvQ":null,"TSup1":18.52,"TSup1Q":null,"TSup2":18.56,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":68,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fee45007-3e8f-41f6-8e56-78f97de6a09f","EventDtm":"2025-11-25T08:34:54Z","AppDtm":"2025-11-25T08:35:10Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:34:54Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":26.60612,"GPSLongitude":80.72381,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.7,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.362Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":69,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6bc867f6-cebf-46ed-87c6-81c89a0973b8","EventDtm":"2025-11-25T08:35:06Z","AppDtm":"2025-11-25T08:35:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:35:06Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.80501,"GPSLongitude":77.662349,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:35:06Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":28.95,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":135.11,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.25,"AmpPhB":10.71,"AmpPhC":10.25,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.08,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.42,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.45,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.12,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.41,"TRtn1Q":null,"TRtn2":5.41,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.83,"PctSucVlvQ":null,"TSup1":5.11,"TSup1Q":null,"TSup2":5.13,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":70,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"355ecb54-e22d-4d4a-a42f-f6a7118a9a2e","EventDtm":"2025-11-25T08:43:35Z","AppDtm":"2025-11-25T08:43:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:43:35Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":26.31057,"GPSLongitude":91.717582,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":45,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:43:35Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":75.8,"TDisQ":null,"FreqComp":null,"TSuc":-24.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1020,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":36,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":392.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":95.43,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.364Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":71,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7a4fcf40-641a-445b-90e6-b76db3a5fee8","EventDtm":"2025-11-25T08:43:36Z","AppDtm":"2025-11-25T08:43:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:43:36Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.80497,"GPSLongitude":77.662296,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:43:36Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.87,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":102.08,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.64,"AmpPhB":10.8,"AmpPhC":11.64,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.25,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.01,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.01,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.83,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.91,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.366Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":72,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"462225f8-5a78-4c09-a0b8-218a08077932","EventDtm":"2025-11-25T08:44:52Z","AppDtm":"2025-11-25T08:45:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:44:52Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.657878,"GPSLongitude":83.101717,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8.1,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:44:52Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":31.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":69.67,"PSucQ":null,"TDis":-190.23,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":130.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.92,"AmpPhB":1.53,"AmpPhC":0.92,"PDis":130.63,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.75,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.05,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.47,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.54,"TRtn1Q":null,"TRtn2":20.59,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":16.99,"PctSucVlvQ":null,"TSup1":19.81,"TSup1Q":null,"TSup2":19.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.367Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":73,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"193e5606-0605-42bc-a3c3-98fe8f2250a7","EventDtm":"2025-11-25T08:50:18Z","AppDtm":"2025-11-25T08:50:39Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:50:18Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.533275,"GPSLongitude":78.433695,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:50:18Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":30.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":77.6,"TDisQ":null,"FreqComp":null,"TSuc":-27.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":416.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.31,"TRtn1Q":null,"TRtn2":6.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.28,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.2,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.368Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":74,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"79d61a39-a2f3-42fa-96aa-3f842271ac43","EventDtm":"2025-11-25T08:53:34Z","AppDtm":"2025-11-25T08:53:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:53:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804961,"GPSLongitude":77.662283,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:53:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.11,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":106.07,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.28,"AmpPhB":11,"AmpPhC":11.28,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.97,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.85,"TRtn1Q":null,"TRtn2":5.87,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.84,"PctSucVlvQ":null,"TSup1":5.06,"TSup1Q":null,"TSup2":4.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.373Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":75,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0fdfaa12-3580-44cd-a5c2-305da6e613d6","EventDtm":"2025-11-25T08:55:14Z","AppDtm":"2025-11-25T08:55:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:55:14Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.539066,"GPSLongitude":78.178316,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:55:14Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":31.5,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":160,"PSucQ":"asProvided","TDis":79.6,"TDisQ":null,"FreqComp":null,"TSuc":-0.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1320,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":42,"PctExpVlvQ":null,"TEvap":2,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":50,"FreqLineQ":null,"VLine1":403,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.12,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":156.1,"PctSucVlvQ":null,"TSup1":3.31,"TSup1Q":null,"TSup2":3.3,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.374Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":76,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"55232bec-6d27-4545-8e15-93c64a084d1d","EventDtm":"2025-11-25T08:56:32Z","AppDtm":"2025-11-25T08:56:49Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:56:32Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":17.67871,"GPSLongitude":78.720186,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8.1,"DeviceTemp":47,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Faulty"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:56:32Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":32.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":230,"PSucQ":"asProvided","TDis":95.6,"TDisQ":null,"FreqComp":null,"TSuc":6.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":820,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":3.5,"TEvapQ":null,"MCtrl3":"EmergencyShutdown","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":88.19,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":391.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"AlarmShutdown","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":14.63,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":803,"RCAlias":"F803","RCSeverity":"Severe","Active":true},{"OemAlarm":107,"RCAlias":"E107","RCSeverity":"Severe","Active":true},{"OemAlarm":809,"RCAlias":"F809","RCSeverity":"Severe","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":77,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9f8f2f00-60bb-402a-9083-4cd6921de0c1","EventDtm":"2025-11-25T08:57:19Z","AppDtm":"2025-11-25T08:57:34Z","Events":["ReeferSwitchOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:57:19Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":26.644585,"GPSLongitude":88.467987,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8.1,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.375Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":78,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0d288ec7-6c65-4c0f-85e6-4ee94abbf7f6","EventDtm":"2025-11-25T08:58:59Z","AppDtm":"2025-11-25T08:59:19Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T08:58:59Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.678732,"GPSLongitude":78.720244,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8.1,"DeviceTemp":46,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Faulty"},"ReeferData":{"ReeferDataDtm":"2025-11-25T08:58:59Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":34.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":230,"PSucQ":"asProvided","TDis":80.2,"TDisQ":null,"FreqComp":null,"TSuc":13.8,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":790,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":4.38,"TEvapQ":null,"MCtrl3":"EmergencyShutdown","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":88.98,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":399.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"AlarmShutdown","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.31,"TSup1Q":null,"TSup2":4.3,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":803,"RCAlias":"F803","RCSeverity":"Severe","Active":true},{"OemAlarm":809,"RCAlias":"F809","RCSeverity":"Severe","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":79,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7dfe0822-49e7-4f09-96b9-5e1e8c92a86e","EventDtm":"2025-11-25T09:00:25Z","AppDtm":"2025-11-25T09:00:42Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:00:25Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.537071,"GPSLongitude":78.175572,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":false,"ExtPowerVoltage":28.2,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":80,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"164c3903-39e7-4380-87de-c5834a16d7ab","EventDtm":"2025-11-25T09:01:12Z","AppDtm":"2025-11-25T09:01:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:01:12Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":21.735738,"GPSLongitude":72.62885,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.9,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:01:12Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":31.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":185.03,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.41,"AmpPhB":12.99,"AmpPhC":13.41,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.34,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90.18,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":430.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.63,"TRtn1Q":null,"TRtn2":15.59,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.99,"PctSucVlvQ":null,"TSup1":14.94,"TSup1Q":null,"TSup2":15.13,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.377Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":81,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c5c494d0-ca53-48af-851b-7149e89057c0","EventDtm":"2025-11-25T09:01:51Z","AppDtm":"2025-11-25T09:02:05Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:01:51Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":26.644612,"GPSLongitude":88.46795,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8.1,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:01:51Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":29.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":170,"PSucQ":"asProvided","TDis":81.1,"TDisQ":null,"FreqComp":null,"TSuc":5.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1600,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":25,"PctExpVlvQ":null,"TEvap":12.88,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":19,"TRtn1Q":null,"TRtn2":18.9,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":12.5,"TSup1Q":null,"TSup2":13.9,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.378Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":82,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9f3d4b0b-964b-47be-8464-100f51b56c8a","EventDtm":"2025-11-25T09:02:27Z","AppDtm":"2025-11-25T09:02:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:02:27Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.82495,"GPSLongitude":78.131531,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:02:27Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":33.69,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":75.4,"TDisQ":null,"FreqComp":null,"TSuc":-21.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1190,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.2,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.379Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":83,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"57ea6712-f370-4e97-aca0-e983d85c93ec","EventDtm":"2025-11-25T09:03:15Z","AppDtm":"2025-11-25T09:03:31Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:03:15Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.537048,"GPSLongitude":78.17554,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":28.5,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:03:15Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":29.5,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":174.33,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":1.43,"AmpPhB":2.58,"AmpPhC":1.43,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.71,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":23.25,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":397.79,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-11.73,"TRtn1Q":null,"TRtn2":-11.69,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":18.72,"PctSucVlvQ":null,"TSup1":-30.03,"TSup1Q":null,"TSup2":-30.71,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.388Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":84,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a518cbaf-b58d-437b-bb4f-814980150eea","EventDtm":"2025-11-25T09:03:34Z","AppDtm":"2025-11-25T09:03:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:03:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804942,"GPSLongitude":77.662244,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:03:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.88,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":109.37,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.51,"AmpPhB":10.93,"AmpPhC":11.51,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.79,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.87,"TRtn1Q":null,"TRtn2":5.89,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.76,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.389Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":85,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a1bd0546-1033-48c7-8d11-51a517353740","EventDtm":"2025-11-25T09:04:49Z","AppDtm":"2025-11-25T09:05:05Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:04:49Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891833,"GPSLongitude":79.475982,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":false,"ExtPowerVoltage":3.6,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":86,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e26fd084-c199-4bf7-8161-e65d927d988f","EventDtm":"2025-11-25T09:05:54Z","AppDtm":"2025-11-25T09:06:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:05:54Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.679138,"GPSLongitude":78.720157,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":43,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:05:54Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":29.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-180.86,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":153.85,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.05,"AmpPhB":10.72,"AmpPhC":11.05,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.51,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.92,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":405.39,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.06,"TRtn1Q":null,"TRtn2":5.06,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.96,"PctSucVlvQ":null,"TSup1":3.97,"TSup1Q":null,"TSup2":3.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T09:14:24.390Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":87,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f959d02a-ff2c-4c81-90a8-2cff8bf212a6","EventDtm":"2025-11-25T10:49:37Z","AppDtm":"2025-11-25T09:08:07Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:49:37Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3938,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34.2,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":88,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"944de7a6-ce6d-4832-90ec-6ffa4d2b892d","EventDtm":"2025-11-25T09:09:11Z","AppDtm":"2025-11-25T09:09:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:09:11Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661646,"GPSLongitude":83.089119,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:09:11Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":31.38,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":130,"PSucQ":"asProvided","TDis":47.5,"TDisQ":null,"FreqComp":null,"TSuc":-1.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1110,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":10,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":363.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.62,"TRtn1Q":null,"TRtn2":5.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":101.83,"PctSucVlvQ":"OOR","TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>{"Sequence":89,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"41efaf20-2f2f-47d5-8e8c-68b0129b0aa1","EventDtm":"2025-11-25T09:12:40Z","AppDtm":"2025-11-25T09:12:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:12:40Z","DeviceID":"JSGA623040302","GPSLockState":"UNLOCKED","GPSSatelliteCount":12,"GPSLastLock":8,"GPSLatitude":19.252845,"GPSLongitude":73.01645,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9f3d4b0b-964b-47be-8464-100f51b56c8a","EventDtm":"2025-11-25T09:02:27Z","AppDtm":"2025-11-25T09:02:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:02:27Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.82495,"GPSLongitude":78.131531,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":44,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:02:27Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":33.69,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":75.4,"TDisQ":null,"FreqComp":null,"TSuc":-21.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1190,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.2,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.422Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"57ea6712-f370-4e97-aca0-e983d85c93ec","EventDtm":"2025-11-25T09:03:15Z","AppDtm":"2025-11-25T09:03:31Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:03:15Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.537048,"GPSLongitude":78.17554,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":28.5,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:03:15Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":29.5,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":174.33,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":1.43,"AmpPhB":2.58,"AmpPhC":1.43,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.71,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":23.25,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":397.79,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-11.73,"TRtn1Q":null,"TRtn2":-11.69,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":18.72,"PctSucVlvQ":null,"TSup1":-30.03,"TSup1Q":null,"TSup2":-30.71,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a518cbaf-b58d-437b-bb4f-814980150eea","EventDtm":"2025-11-25T09:03:34Z","AppDtm":"2025-11-25T09:03:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:03:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":12.804942,"GPSLongitude":77.662244,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:03:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.88,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":109.37,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.51,"AmpPhB":10.93,"AmpPhC":11.51,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.79,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.87,"TRtn1Q":null,"TRtn2":5.89,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.76,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.436Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a1bd0546-1033-48c7-8d11-51a517353740","EventDtm":"2025-11-25T09:04:49Z","AppDtm":"2025-11-25T09:05:05Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:04:49Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891833,"GPSLongitude":79.475982,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":false,"ExtPowerVoltage":3.6,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.439Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e26fd084-c199-4bf7-8161-e65d927d988f","EventDtm":"2025-11-25T09:05:54Z","AppDtm":"2025-11-25T09:06:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:05:54Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.679138,"GPSLongitude":78.720157,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":43,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:05:54Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":29.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-180.86,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":153.85,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.05,"AmpPhB":10.72,"AmpPhC":11.05,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.51,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.92,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":405.39,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.04,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.06,"TRtn1Q":null,"TRtn2":5.06,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.96,"PctSucVlvQ":null,"TSup1":3.97,"TSup1Q":null,"TSup2":3.99,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f959d02a-ff2c-4c81-90a8-2cff8bf212a6","EventDtm":"2025-11-25T10:49:37Z","AppDtm":"2025-11-25T09:08:07Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:49:37Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3938,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34.2,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.597Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"944de7a6-ce6d-4832-90ec-6ffa4d2b892d","EventDtm":"2025-11-25T09:09:11Z","AppDtm":"2025-11-25T09:09:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:09:11Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.661646,"GPSLongitude":83.089119,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.8,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:09:11Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":31.38,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":130,"PSucQ":"asProvided","TDis":47.5,"TDisQ":null,"FreqComp":null,"TSuc":-1.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1110,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":10,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":363.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.62,"TRtn1Q":null,"TRtn2":5.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":101.83,"PctSucVlvQ":"OOR","TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.605Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"41efaf20-2f2f-47d5-8e8c-68b0129b0aa1","EventDtm":"2025-11-25T09:12:40Z","AppDtm":"2025-11-25T09:12:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:12:40Z","DeviceID":"JSGA623040302","GPSLockState":"UNLOCKED","GPSSatelliteCount":12,"GPSLastLock":8,"GPSLatitude":19.252845,"GPSLongitude":73.01645,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.609Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"506a4489-3fda-4f3c-96d2-206f3e901692","EventDtm":"2025-11-25T09:13:34Z","AppDtm":"2025-11-25T09:13:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:13:34Z","DeviceID":"JSGA623040329","GPSLockState":"LOCKED","GPSSatelliteCount":7,"GPSLastLock":1,"GPSLatitude":17.548036,"GPSLongitude":78.38087,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.610Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9d4e106d-efc8-4f9c-b5b1-5877b7418fb8","EventDtm":"2025-11-25T09:13:39Z","AppDtm":"2025-11-25T09:13:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:13:39Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.805077,"GPSLongitude":77.662302,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:13:39Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.98,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":103.62,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.51,"AmpPhB":10.82,"AmpPhC":11.51,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.96,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.02,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.81,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.8,"PctSucVlvQ":null,"TSup1":4.98,"TSup1Q":null,"TSup2":4.9,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.614Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fb8e677d-dcec-423e-a811-7fd09e44ed29","EventDtm":"2025-11-25T09:17:23Z","AppDtm":"2025-11-25T09:17:43Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:17:23Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":15.47947,"GPSLongitude":73.969704,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":4.4,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.615Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"718da110-9000-4320-9bc6-70df53e69ea8","EventDtm":"2025-11-25T09:17:35Z","AppDtm":"2025-11-25T09:17:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:17:35Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.547775,"GPSLongitude":78.380496,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.616Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"db48d890-8a4d-41d0-b5fe-43ff1fb3fe1d","EventDtm":"2025-11-25T09:18:04Z","AppDtm":"2025-11-25T09:18:20Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:18:04Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":16.891862,"GPSLongitude":79.475936,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:18:04Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":30.81,"TAmbQ":null,"TUSDA4":-53.2,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":260,"PSucQ":"asProvided","TDis":42.8,"TDisQ":null,"FreqComp":null,"TSuc":10.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.12,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":7.69,"TRtn1Q":null,"TRtn2":7.7,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":0,"PctSucVlvQ":null,"TSup1":5.62,"TSup1Q":null,"TSup2":5.4,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.2,"TUSDA1Q":"OOR","TUSDA2":-53,"TUSDA2Q":"OOR","TUSDA3":-53.1,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.617Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"df2f7184-fbf8-42be-88a3-e08ed3b5200c","EventDtm":"2025-11-25T09:18:53Z","AppDtm":"2025-11-25T09:19:07Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:18:53Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":15.479474,"GPSLongitude":73.969655,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":28.8,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:18:53Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.75,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":2,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":141.03,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":2.34,"AmpPhB":2.17,"AmpPhC":2.34,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":7.29,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":81.87,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.52,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":1.31,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":7.14,"TRtn1Q":null,"TRtn2":7.17,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":17.77,"PctSucVlvQ":null,"TSup1":6.19,"TSup1Q":null,"TSup2":6.21,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.619Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8dabda7f-a529-472f-9a52-60ebdb53d153","EventDtm":"2025-11-25T09:19:12Z","AppDtm":"2025-11-25T09:19:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:19:12Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.57222,"GPSLongitude":78.515068,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323415","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.623Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e40a45c9-4ca1-45f9-8ba9-2b8d9d565708","EventDtm":"2025-11-25T09:19:15Z","AppDtm":"2025-11-25T09:19:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:19:15Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.67873,"GPSLongitude":78.720259,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.8,"BatteryVoltage":8.1,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Faulty"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:19:15Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":39.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":250,"PSucQ":"asProvided","TDis":45.8,"TDisQ":null,"FreqComp":null,"TSuc":33.3,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":710,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":6.31,"TEvapQ":null,"MCtrl3":"EmergencyShutdown","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":81.1,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"AlarmShutdown","TRtn1":7.5,"TRtn1Q":null,"TRtn2":7.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":7.69,"TSup1Q":null,"TSup2":7.6,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":803,"RCAlias":"F803","RCSeverity":"Severe","Active":true},{"OemAlarm":809,"RCAlias":"F809","RCSeverity":"Severe","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.624Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0c9a44e1-4a33-4124-ae04-c122137bcf54","EventDtm":"2025-11-25T09:19:26Z","AppDtm":"2025-11-25T09:19:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:19:26Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.892147,"GPSLongitude":79.476234,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:19:26Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":30.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":83.9,"TDisQ":null,"FreqComp":null,"TSuc":-27.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":-0.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.2,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.625Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5cdc4489-7e01-4d2e-bb8a-f3355189d12d","EventDtm":"2025-11-25T09:20:13Z","AppDtm":"2025-11-25T09:20:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:20:13Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.533223,"GPSLongitude":78.433029,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8.1,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Standby"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.627Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a04ba08b-ca8e-4da7-84de-71945cf7bd38","EventDtm":"2025-11-25T09:21:34Z","AppDtm":"2025-11-25T09:21:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:21:34Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.516221,"GPSLongitude":82.962345,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":"-53","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:21:34Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":29.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":80.6,"TDisQ":null,"FreqComp":null,"TSuc":-11.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":850,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":53,"PctExpVlvQ":null,"TEvap":22.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":384.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.7,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.67,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.629Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fcceb0df-8776-4e72-88f4-0ae400dbb126","EventDtm":"2025-11-25T09:23:35Z","AppDtm":"2025-11-25T09:23:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:23:35Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.80503,"GPSLongitude":77.662247,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:23:35Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.63,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":101.91,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.42,"AmpPhB":10.83,"AmpPhC":11.42,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.25,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.61,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.03,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.82,"TRtn1Q":null,"TRtn2":5.84,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.09,"PctSucVlvQ":null,"TSup1":5.03,"TSup1Q":null,"TSup2":4.94,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.637Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"32ae9b8e-466d-4e69-b982-189cac23859f","EventDtm":"2025-11-25T09:25:24Z","AppDtm":"2025-11-25T09:25:39Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:25:24Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":16.891835,"GPSLongitude":79.475897,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:25:24Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":32.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":280,"PSucQ":"asProvided","TDis":50.7,"TDisQ":null,"FreqComp":null,"TSuc":8.3,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":38,"PctExpVlvQ":null,"TEvap":7,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":406.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":7.69,"TRtn1Q":null,"TRtn2":37.6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":89.33,"PctSucVlvQ":null,"TSup1":7,"TSup1Q":null,"TSup2":6.8,"TSup2Q":null,"AmpTotalDraw":3,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.638Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3ec38153-bede-4785-971f-ab18433e73cf","EventDtm":"2025-11-25T09:24:02Z","AppDtm":"2025-11-25T09:25:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:24:02Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":28.364696,"GPSLongitude":75.581346,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-85","ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:24:02Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":24,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":36,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":5.3,"AmpPhB":6.2,"AmpPhC":6,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":400,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.3,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":8.8,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.807Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"76c1465b-0420-4d40-b02e-a937c56d5705","EventDtm":"2025-11-25T09:25:52Z","AppDtm":"2025-11-25T09:26:09Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:25:52Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":17.516049,"GPSLongitude":82.981156,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":37,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:25:52Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":29.81,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":137.7,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.07,"AmpPhB":10.74,"AmpPhC":11.07,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":4.04,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":95.51,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":405.93,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.15,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.75,"TRtn1Q":null,"TRtn2":3.79,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":5.21,"PctSucVlvQ":null,"TSup1":2.86,"TSup1Q":null,"TSup2":2.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.816Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":24,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f35283ab-eddf-406f-8a69-40339884980f","EventDtm":"2025-11-25T11:11:04Z","AppDtm":"2025-11-25T09:29:33Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:11:04Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3960,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":false,"ExtPowerVoltage":34.3,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.817Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":25,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"583cf4df-2e00-47fe-a5b5-ef662bcc810a","EventDtm":"2025-11-25T09:30:07Z","AppDtm":"2025-11-25T09:30:28Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:30:07Z","DeviceID":"JSGA623040314","GPSLockState":"UNLOCKED","GPSSatelliteCount":11,"GPSLastLock":16,"GPSLatitude":19.252979,"GPSLongitude":73.016372,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":28.6,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:30:07Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":32.41,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.23,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":155.34,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.42,"AmpPhB":10.61,"AmpPhC":10.42,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.85,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":391.3,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.12,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.35,"TRtn1Q":null,"TRtn2":5.49,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":4.23,"PctSucVlvQ":null,"TSup1":7.88,"TSup1Q":null,"TSup2":4.88,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":26,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"49c69e12-4e5f-44b4-ab17-167ee744b94e","EventDtm":"2025-11-25T09:32:40Z","AppDtm":"2025-11-25T09:32:58Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:32:40Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":28.678905,"GPSLongitude":77.599625,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":28.7,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:32:40Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":23.61,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":67.68,"PSucQ":null,"TDis":30.55,"TDisQ":null,"FreqComp":null,"TSuc":21.29,"TSucQ":null,"MCond":0,"PCond":295.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04475864","AmpPhA":0,"AmpPhB":0,"AmpPhC":0,"PDis":91.04,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":22.03,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":62.71,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.84,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":22.42,"TRtn1Q":null,"TRtn2":22.42,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":21.06,"TSup1Q":null,"TSup2":20.95,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.818Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":27,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"16e3ff1b-f3d6-4665-85c1-9745b7e78d53","EventDtm":"2025-11-25T09:33:34Z","AppDtm":"2025-11-25T09:33:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:33:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":12.805016,"GPSLongitude":77.662224,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:33:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.45,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":111.68,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.49,"AmpPhB":10.9,"AmpPhC":11.49,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.29,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.11,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.12,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.86,"TRtn1Q":null,"TRtn2":5.88,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.4,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.05,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":28,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5cb78496-e0fd-4ac9-92ef-a2e4efb35db6","EventDtm":"2025-11-25T09:34:52Z","AppDtm":"2025-11-25T09:35:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:34:52Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":26.606151,"GPSLongitude":80.723639,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.819Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":29,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"cba310ad-1ef0-43cd-b2e0-b66cb689f90c","EventDtm":"2025-11-25T09:34:56Z","AppDtm":"2025-11-25T09:35:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:34:56Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.657898,"GPSLongitude":83.101712,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":7.9,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:34:56Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":29.83,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":69.49,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":124.09,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.9,"AmpPhB":1.53,"AmpPhC":0.9,"PDis":140.4,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":405.89,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.69,"TRtn1Q":null,"TRtn2":20.73,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":18.49,"PctSucVlvQ":null,"TSup1":20.46,"TSup1Q":null,"TSup2":20.47,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.820Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":30,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b2c83879-1418-4bb6-8ef5-82d0569f25bf","EventDtm":"2025-11-25T09:35:09Z","AppDtm":"2025-11-25T09:35:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:35:09Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.892124,"GPSLongitude":79.476192,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:35:09Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":32.37,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-192.19,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":158.45,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":10.99,"AmpPhB":10.88,"AmpPhC":10.99,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.06,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.21,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.81,"TRtn1Q":null,"TRtn2":17.74,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.16,"PctSucVlvQ":null,"TSup1":18.49,"TSup1Q":null,"TSup2":18.52,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.821Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":31,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"552332ae-30cb-41ed-a6a3-f3078bd2ace1","EventDtm":"2025-11-25T09:35:15Z","AppDtm":"2025-11-25T09:35:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:35:15Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804994,"GPSLongitude":77.662218,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:35:15Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":29.44,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":186.05,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.11,"AmpPhB":10.56,"AmpPhC":10.11,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.04,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.42,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.31,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.04,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.37,"TRtn1Q":null,"TRtn2":5.38,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":3.49,"PctSucVlvQ":null,"TSup1":5.02,"TSup1Q":null,"TSup2":5.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":32,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b59ee3cb-0d00-4e68-aba9-c2103abd1a13","EventDtm":"2025-11-25T09:35:31Z","AppDtm":"2025-11-25T09:35:52Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:35:31Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.678754,"GPSLongitude":78.720168,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8.1,"DeviceTemp":49,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:35:31Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":38.19,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":290,"PSucQ":"asProvided","TDis":40.6,"TDisQ":null,"FreqComp":null,"TSuc":37.4,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":460,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":7.38,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":75.98,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":393.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":9,"TRtn1Q":null,"TRtn2":8.7,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":9.19,"TSup1Q":null,"TSup2":9.3,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.823Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":33,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2b1605dd-65ad-468e-b4f9-d49396d032fd","EventDtm":"2025-11-25T09:34:25Z","AppDtm":"2025-11-25T09:36:23Z","Events":["DeviceIsStationary"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:34:25Z","DeviceID":"JSGA622340507","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":17.50238,"GPSLongitude":82.961991,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"233175553","RSSI":null,"ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.7,"DeviceTemp":40,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6616969","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.824Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":34,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"98d16ed4-60ef-44a1-bf44-2f21f1a36fd2","EventDtm":"2025-11-25T09:40:09Z","AppDtm":"2025-11-25T09:40:24Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:40:09Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":26.310614,"GPSLongitude":91.717588,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":false,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":35,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ef79eb05-9871-45ff-a8b8-08fd013bd33d","EventDtm":"2025-11-25T09:41:42Z","AppDtm":"2025-11-25T09:41:57Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:41:42Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":21,"GPSLastLock":0,"GPSLatitude":26.310619,"GPSLongitude":91.717573,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.4,"BatteryVoltage":8,"DeviceTemp":38,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.825Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":36,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9c4bee5c-e2dd-4fa8-a890-5b8c140b3825","EventDtm":"2025-11-25T09:43:34Z","AppDtm":"2025-11-25T09:43:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:43:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804958,"GPSLongitude":77.662164,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.1,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:43:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.87,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":104.97,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.09,"AmpPhB":10.9,"AmpPhC":11.09,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.22,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":409.67,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.09,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.8,"TRtn1Q":null,"TRtn2":5.82,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.06,"PctSucVlvQ":null,"TSup1":4.9,"TSup1Q":null,"TSup2":4.82,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":37,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"fd0592d4-29f4-4d30-996d-98e5666b115a","EventDtm":"2025-11-25T11:26:05Z","AppDtm":"2025-11-25T09:44:38Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:26:05Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3975,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.826Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":38,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d64c35cf-70e8-41a5-a107-3c9757e98962","EventDtm":"2025-11-25T09:44:27Z","AppDtm":"2025-11-25T09:44:41Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:44:27Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":26.310619,"GPSLongitude":91.717587,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8,"DeviceTemp":40,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:44:27Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":30.12,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":250,"PSucQ":"asProvided","TDis":53.2,"TDisQ":null,"FreqComp":null,"TSuc":4.5,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":240,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":50,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"PTIEmergencyStop1","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":404.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":45.19,"TRtn1Q":null,"TRtn2":5.9,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":46.65,"PctSucVlvQ":null,"TSup1":5.5,"TSup1Q":null,"TSup2":5.3,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.828Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":39,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1dec1ef1-8b87-4fe3-a49c-d41771674bae","EventDtm":"2025-11-25T09:44:40Z","AppDtm":"2025-11-25T09:44:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:44:40Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.657864,"GPSLongitude":83.101753,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":28.4,"BatteryVoltage":8.1,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:44:40Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":31.04,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":48.98,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":109.12,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04783085","AmpPhA":13.3,"AmpPhB":13.48,"AmpPhC":13.3,"PDis":164.18,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.49,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":399.23,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":21,"TRtn1Q":null,"TRtn2":21.07,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":23.96,"PctSucVlvQ":null,"TSup1":21.36,"TSup1Q":null,"TSup2":21.43,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.831Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":40,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"98ccaef3-1024-43f2-95ee-c49343ead837","EventDtm":"2025-11-25T11:26:06Z","AppDtm":"2025-11-25T09:44:59Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:26:06Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3975,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":false,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.833Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":41,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"e7193b38-f2fc-4d24-af3c-00fd66146507","EventDtm":"2025-11-25T11:27:06Z","AppDtm":"2025-11-25T09:45:38Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:27:06Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3976,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.834Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":42,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1a0843aa-14b2-410e-9927-4fc684045851","EventDtm":"2025-11-25T09:45:32Z","AppDtm":"2025-11-25T09:45:48Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:45:32Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":22,"GPSLastLock":0,"GPSLatitude":26.310635,"GPSLongitude":91.717613,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":40,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:45:32Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":30.19,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":160,"PSucQ":"asProvided","TDis":51.4,"TDisQ":null,"FreqComp":null,"TSuc":4.3,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1300,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":100,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":405,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":6.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":109.15,"PctSucVlvQ":null,"TSup1":5.69,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.835Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":43,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4f5248a7-8b72-4c77-92ba-a673d998ac67","EventDtm":"2025-11-25T11:27:06Z","AppDtm":"2025-11-25T09:46:11Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:27:06Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3976,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":false,"ExtPowerVoltage":5.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":44,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2d48a3d3-5249-41e5-9f33-1227ce93b3f2","EventDtm":"2025-11-25T11:30:57Z","AppDtm":"2025-11-25T09:49:25Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:30:57Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3979,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":6.8,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.836Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":45,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7132801e-8e27-45a7-b415-243ac8618aa0","EventDtm":"2025-11-25T11:30:57Z","AppDtm":"2025-11-25T09:49:35Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:30:57Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3979,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":false,"ExtPowerVoltage":6.8,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":46,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c24e3be9-c46f-4f84-b239-212e7cacbeb0","EventDtm":"2025-11-25T11:31:57Z","AppDtm":"2025-11-25T09:50:25Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:31:57Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3980,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":4,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.837Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":47,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"242396b3-1da3-4a6e-9481-1b256500c3e7","EventDtm":"2025-11-25T11:31:57Z","AppDtm":"2025-11-25T09:50:34Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:31:57Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3980,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":false,"ExtPowerVoltage":4,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":48,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3b64e599-f99b-4b18-b2cf-03240395a8eb","EventDtm":"2025-11-25T09:50:29Z","AppDtm":"2025-11-25T09:50:48Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:50:29Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.533219,"GPSLongitude":78.433624,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:50:29Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":30.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":77,"TDisQ":null,"FreqComp":null,"TSuc":-28.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":411,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.31,"TRtn1Q":null,"TRtn2":6.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.2,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.838Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":49,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"33dd0641-bb9e-4304-a23e-706055230472","EventDtm":"2025-11-25T09:53:37Z","AppDtm":"2025-11-25T09:53:51Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:53:37Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.804933,"GPSLongitude":77.662155,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:53:37Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.7,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":2,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":138.24,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":15.19,"AmpPhB":14.22,"AmpPhC":15.19,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":7.84,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.93,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.74,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":7.39,"TRtn1Q":null,"TRtn2":7.39,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.55,"PctSucVlvQ":null,"TSup1":6.1,"TSup1Q":null,"TSup2":6.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":50,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"23f95bfe-73c8-487a-a9ea-efc554d8a5bc","EventDtm":"2025-11-25T09:55:19Z","AppDtm":"2025-11-25T09:55:34Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T09:55:19Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":17.539015,"GPSLongitude":78.178234,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T09:55:19Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":29.81,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":110,"TDisQ":null,"FreqComp":null,"TSuc":-32.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":960,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":401.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.19,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":92.38,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.841Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":51,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c0b02343-0245-465c-904d-dd601eeb94ac","EventDtm":"2025-11-25T10:01:10Z","AppDtm":"2025-11-25T10:01:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:01:10Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":21.735525,"GPSLongitude":72.628957,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":30.5,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:01:10Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":32.51,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":191.06,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.58,"AmpPhB":13.03,"AmpPhC":13.58,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.28,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90.19,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":431.81,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.13,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.57,"TRtn1Q":null,"TRtn2":15.53,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":1.69,"PctSucVlvQ":null,"TSup1":14.87,"TSup1Q":null,"TSup2":15.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.842Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":52,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a8c85bc9-621a-43dd-99e7-3ca76ca7f9e9","EventDtm":"2025-11-25T10:01:52Z","AppDtm":"2025-11-25T10:02:06Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:01:52Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":26.644596,"GPSLongitude":88.468053,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33,"BatteryVoltage":8.1,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:01:52Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":28.69,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":100,"PSucQ":"asProvided","TDis":89,"TDisQ":null,"FreqComp":null,"TSuc":6.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1300,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":24,"PctExpVlvQ":null,"TEvap":1.69,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4,"TRtn1Q":null,"TRtn2":4.6,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":1.12,"TSup1Q":null,"TSup2":2.7,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:31.843Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":53,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"c3e77c17-ca43-4a57-aa90-377f4fedd099","EventDtm":"2025-11-25T10:02:30Z","AppDtm":"2025-11-25T10:02:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:02:30Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.824916,"GPSLongitude":78.131506,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.6,"BatteryVoltage":8,"DeviceTemp":41,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:02:30Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":32.69,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":75.4,"TDisQ":null,"FreqComp":null,"TSuc":-22.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1140,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":394.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":11.89,"PctSucVlvQ":null,"TSup1":5.12,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":16,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.007Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":54,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d0bc33b6-abf9-43e3-badc-645a38cf0819","EventDtm":"2025-11-25T10:02:49Z","AppDtm":"2025-11-25T10:03:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:02:49Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.537159,"GPSLongitude":78.175653,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":27.3,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:02:49Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":28.88,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":131.2,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":10.27,"AmpPhB":10.63,"AmpPhC":10.27,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-20.43,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":61.39,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":388.13,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-13.58,"TRtn1Q":null,"TRtn2":-13.62,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-26.52,"TSup1Q":null,"TSup2":-25.32,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.018Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":55,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9c66df14-2e55-4b84-aea0-d37f4620c3e3","EventDtm":"2025-11-25T10:03:37Z","AppDtm":"2025-11-25T10:03:53Z","Events":["ReeferSwitchOff"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:03:37Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.533152,"GPSLongitude":78.433525,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":41,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Standby"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:03:37Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":30.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":160,"PSucQ":"asProvided","TDis":79.3,"TDisQ":null,"FreqComp":null,"TSuc":-9.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":940,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.69,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":410.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":7,"TRtn1Q":null,"TRtn2":7.1,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":17.68,"PctSucVlvQ":null,"TSup1":5.5,"TSup1Q":null,"TSup2":5.4,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":56,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ca841ca2-9b18-4417-bcf5-b1a9c890fd4c","EventDtm":"2025-11-25T10:03:34Z","AppDtm":"2025-11-25T10:04:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:03:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804962,"GPSLongitude":77.662203,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:03:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":33.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":118.32,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.92,"AmpPhB":11.55,"AmpPhC":11.92,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.72,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.65,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.46,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":6.48,"TRtn1Q":null,"TRtn2":6.49,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":4.56,"TSup1Q":null,"TSup2":4.5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.019Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":57,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5a9823b2-6302-4d71-a194-0e167cea92b1","EventDtm":"2025-11-25T11:46:39Z","AppDtm":"2025-11-25T10:05:08Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:46:39Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3995,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":58,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"71b34242-be14-4ef1-aed5-b36f6d987fff","EventDtm":"2025-11-25T10:06:01Z","AppDtm":"2025-11-25T10:06:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:06:01Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.679109,"GPSLongitude":78.72022,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:06:01Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":28.36,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.42,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":149.83,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.36,"AmpPhB":10.98,"AmpPhC":11.36,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.44,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":99.32,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":412.15,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.05,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5,"TRtn1Q":null,"TRtn2":4.99,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.67,"PctSucVlvQ":null,"TSup1":3.93,"TSup1Q":null,"TSup2":3.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":59,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1f4283b1-509d-4ba0-a4fb-0403feb3de77","EventDtm":"2025-11-25T11:49:01Z","AppDtm":"2025-11-25T10:07:28Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:49:01Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3998,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":false,"ExtPowerVoltage":33.7,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":60,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1c0ea30c-f6bb-4371-91b7-ffe62e007e05","EventDtm":"2025-11-25T10:08:49Z","AppDtm":"2025-11-25T10:09:06Z","Events":["ReeferSwitchOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:08:49Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533107,"GPSLongitude":78.433423,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":41,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.021Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":61,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"74b29881-a41d-4517-8162-c2f54e031ec0","EventDtm":"2025-11-25T10:09:09Z","AppDtm":"2025-11-25T10:09:29Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:09:09Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.661684,"GPSLongitude":83.089055,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:09:09Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":31.19,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":60,"PSucQ":"asProvided","TDis":47.7,"TDisQ":null,"FreqComp":null,"TSuc":-12.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1100,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":360.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.5,"TRtn1Q":null,"TRtn2":5.4,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":100.91,"PctSucVlvQ":"OOR","TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":62,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"93d0f64f-ac48-4af1-9af7-02038c103ade","EventDtm":"2025-11-25T10:10:55Z","AppDtm":"2025-11-25T10:11:26Z","Events":["ReeferSwitchOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:10:55Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.533274,"GPSLongitude":78.433045,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.3,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.031Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":63,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"31f445c8-d1ef-49d7-8dbd-3188ebfd24d4","EventDtm":"2025-11-25T10:11:17Z","AppDtm":"2025-11-25T10:11:53Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:11:17Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.533232,"GPSLongitude":78.433055,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.6,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:11:17Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":27.62,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":420,"PSucQ":"asProvided","TDis":27.7,"TDisQ":null,"FreqComp":null,"TSuc":26.6,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":420,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":46.85,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":412.9,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":19.88,"TRtn1Q":null,"TRtn2":135.7,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":57.93,"PctSucVlvQ":null,"TSup1":18.38,"TSup1Q":null,"TSup2":18.5,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.2,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":64,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"90c160a6-52e6-4154-9109-188f88fa5695","EventDtm":"2025-11-25T10:13:01Z","AppDtm":"2025-11-25T10:13:17Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:13:01Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":2,"GPSLatitude":19.252889,"GPSLongitude":73.016429,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":28.6,"BatteryVoltage":8,"DeviceTemp":39,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.032Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":65,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"663ea5f9-ae2b-4ebe-92be-fbf030560d4b","EventDtm":"2025-11-25T10:13:34Z","AppDtm":"2025-11-25T10:13:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:13:34Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":12.804976,"GPSLongitude":77.662177,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:13:34Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":32.77,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":105.2,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.33,"AmpPhB":11.06,"AmpPhC":11.33,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.41,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.71,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.19,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":6.02,"TRtn1Q":null,"TRtn2":6.03,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.26,"PctSucVlvQ":null,"TSup1":4.82,"TSup1Q":null,"TSup2":4.77,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":66,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"625fdcb5-01d8-4952-93b4-c116a598e139","EventDtm":"2025-11-25T10:13:31Z","AppDtm":"2025-11-25T10:13:51Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:13:31Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.533273,"GPSLongitude":78.433067,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:13:31Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":28.5,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":260,"PSucQ":"asProvided","TDis":67.8,"TDisQ":null,"FreqComp":null,"TSuc":8.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1740,"PDisQ":"asProvided","PctEconVlv":100,"PctEconVlvQ":null,"PctExpVlv":50,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":40.16,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":17,"TRtn1Q":null,"TRtn2":135.9,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":142.38,"PctSucVlvQ":null,"TSup1":12.88,"TSup1Q":null,"TSup2":12.9,"TSup2Q":null,"AmpTotalDraw":17,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.2,"TUSDA1Q":"OOR","TUSDA2":-46.2,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:17:32.033Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":67,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b3676a43-c987-4370-b8ee-b2a324e958a8","EventDtm":"2025-11-25T10:13:43Z","AppDtm":"2025-11-25T10:13:58Z","Events":["ReeferSwitchOff"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:13:43Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.533105,"GPSLongitude":78.433502,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8,"DeviceTemp":41,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Standby"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":68,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ab9c21fd-8f18-40c7-926a-1dd4a434b9f5","EventDtm":"2025-11-25T10:14:10Z","AppDtm":"2025-11-25T10:14:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:14:10Z","DeviceID":"JSGA623040329","GPSLockState":"LOCKED","GPSSatelliteCount":8,"GPSLastLock":1,"GPSLatitude":17.548016,"GPSLongitude":78.380524,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>{"Sequence":69,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d3f3504c-62e0-404f-9dc1-19662826f447","EventDtm":"2025-11-25T10:14:02Z","AppDtm":"2025-11-25T10:15:57Z","Events":["DeviceIsMoving"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:14:02Z","DeviceID":"JSGA622180064","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":0,"GPSLatitude":17.537878,"GPSLongitude":78.234398,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232146996","RSSI":"-59","ExtPower":false,"ExtPowerVoltage":0,"BatteryVoltage":7.4,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1041571","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:18:01.334Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":70,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d0ff5efa-1337-4425-96e7-c1f1d69573c3","EventDtm":"2025-11-25T10:17:40Z","AppDtm":"2025-11-25T10:18:01Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:17:40Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.547704,"GPSLongitude":78.380596,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.8,"BatteryVoltage":8.1,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:18:15.134Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":71,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8880a97a-245f-40fc-a7b2-98318283c4c1","EventDtm":"2025-11-25T11:59:43Z","AppDtm":"2025-11-25T10:18:14Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T11:59:43Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":4008,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:18:15.330Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":72,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b7f23c06-251b-4a43-9943-a6f0255854a4","EventDtm":"2025-11-25T10:17:56Z","AppDtm":"2025-11-25T10:18:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:17:56Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":16.891819,"GPSLongitude":79.475959,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31.7,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:17:56Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":30.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":68.6,"TDisQ":null,"FreqComp":null,"TSuc":-27.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1000,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":399.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.69,"TRtn1Q":null,"TRtn2":37.5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:18:44.562Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":73,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d6005aa5-b6fa-456a-8e83-b02d49c51394","EventDtm":"2025-11-25T10:18:29Z","AppDtm":"2025-11-25T10:18:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:18:29Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":15.47951,"GPSLongitude":73.969695,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.3,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:18:29Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":30.29,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":153.79,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.63,"AmpPhB":10.15,"AmpPhC":10.63,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.01,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.45,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.91,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.63,"TRtn1Q":null,"TRtn2":5.65,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.35,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:19:32.918Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":74,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"51bc92d1-eae6-432e-9500-0ffdc15164db","EventDtm":"2025-11-25T10:19:19Z","AppDtm":"2025-11-25T10:19:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:19:19Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":19,"GPSLastLock":0,"GPSLatitude":17.572267,"GPSLongitude":78.51505,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323415","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:19:40.567Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":75,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"56e3727e-41b0-4e59-9185-cb270f2f4d4a","EventDtm":"2025-11-25T10:19:23Z","AppDtm":"2025-11-25T10:19:40Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:19:23Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.678813,"GPSLongitude":78.720108,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31,"BatteryVoltage":8.1,"DeviceTemp":42,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:19:23Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":30.19,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":10,"PSucQ":"asProvided","TDis":91.7,"TDisQ":null,"FreqComp":null,"TSuc":4.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":2.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":88.98,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":394,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":13.72,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:19:46.286Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":76,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"64f9de8b-ee9a-46d5-8b46-225e7bc3d076","EventDtm":"2025-11-25T10:19:31Z","AppDtm":"2025-11-25T10:19:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:19:31Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892112,"GPSLongitude":79.476208,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8,"DeviceTemp":36,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:19:31Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":30.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":84,"TDisQ":null,"FreqComp":null,"TSuc":-27.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":-0.69,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":398.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.62,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.2,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T10:20:35.938Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":77,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"363e972f-e325-47b1-a299-af5de86b6e38","EventDtm":"2025-11-25T10:20:19Z","AppDtm":"2025-11-25T10:20:35Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T10:20:19Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.533187,"GPSLongitude":78.43304,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"231571714","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8.1,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T10:20:19Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":29.88,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":170,"PSucQ":"asProvided","TDis":82.2,"TDisQ":null,"FreqComp":null,"TSuc":10.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1470,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":34,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"FullCool","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":29.92,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"CoolMax","TRtn1":13.81,"TRtn1Q":null,"TRtn2":136.1,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":125,"PctSucVlvQ":null,"TSup1":9.31,"TSup1Q":null,"TSup2":9.6,"TSup2Q":null,"AmpTotalDraw":15,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
   </si>
 </sst>
 </file>
@@ -912,7 +834,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1029,103 +951,103 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -1152,12 +1074,12 @@
         <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -1184,12 +1106,12 @@
         <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1216,12 +1138,12 @@
         <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1248,12 +1170,12 @@
         <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1280,12 +1202,12 @@
         <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -1312,12 +1234,12 @@
         <v>11</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -1344,12 +1266,12 @@
         <v>11</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -1376,12 +1298,12 @@
         <v>11</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1408,12 +1330,12 @@
         <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
@@ -1440,12 +1362,12 @@
         <v>11</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
@@ -1472,12 +1394,12 @@
         <v>11</v>
       </c>
       <c r="J17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -1504,12 +1426,12 @@
         <v>11</v>
       </c>
       <c r="J18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -1536,12 +1458,12 @@
         <v>11</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1568,12 +1490,12 @@
         <v>11</v>
       </c>
       <c r="J20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -1600,12 +1522,12 @@
         <v>11</v>
       </c>
       <c r="J21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -1632,12 +1554,12 @@
         <v>11</v>
       </c>
       <c r="J22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>11</v>
@@ -1664,12 +1586,12 @@
         <v>11</v>
       </c>
       <c r="J23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
@@ -1696,12 +1618,12 @@
         <v>11</v>
       </c>
       <c r="J24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
@@ -1728,12 +1650,12 @@
         <v>11</v>
       </c>
       <c r="J25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
@@ -1760,12 +1682,12 @@
         <v>11</v>
       </c>
       <c r="J26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
@@ -1792,12 +1714,12 @@
         <v>11</v>
       </c>
       <c r="J27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -1824,12 +1746,12 @@
         <v>11</v>
       </c>
       <c r="J28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -1856,12 +1778,12 @@
         <v>11</v>
       </c>
       <c r="J29" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1888,12 +1810,12 @@
         <v>11</v>
       </c>
       <c r="J30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
@@ -1920,12 +1842,12 @@
         <v>11</v>
       </c>
       <c r="J31" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
@@ -1952,12 +1874,12 @@
         <v>11</v>
       </c>
       <c r="J32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
@@ -1984,12 +1906,12 @@
         <v>11</v>
       </c>
       <c r="J33" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
@@ -2016,12 +1938,12 @@
         <v>11</v>
       </c>
       <c r="J34" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
@@ -2048,12 +1970,12 @@
         <v>11</v>
       </c>
       <c r="J35" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
@@ -2080,12 +2002,12 @@
         <v>11</v>
       </c>
       <c r="J36" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -2112,12 +2034,12 @@
         <v>11</v>
       </c>
       <c r="J37" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -2144,12 +2066,12 @@
         <v>11</v>
       </c>
       <c r="J38" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
@@ -2176,12 +2098,12 @@
         <v>11</v>
       </c>
       <c r="J39" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
@@ -2208,12 +2130,12 @@
         <v>11</v>
       </c>
       <c r="J40" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
         <v>11</v>
@@ -2240,12 +2162,12 @@
         <v>11</v>
       </c>
       <c r="J41" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -2272,12 +2194,12 @@
         <v>11</v>
       </c>
       <c r="J42" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
@@ -2304,12 +2226,12 @@
         <v>11</v>
       </c>
       <c r="J43" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
@@ -2336,12 +2258,12 @@
         <v>11</v>
       </c>
       <c r="J44" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
         <v>11</v>
@@ -2368,12 +2290,12 @@
         <v>11</v>
       </c>
       <c r="J45" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -2400,12 +2322,12 @@
         <v>11</v>
       </c>
       <c r="J46" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -2432,12 +2354,12 @@
         <v>11</v>
       </c>
       <c r="J47" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
         <v>11</v>
@@ -2464,12 +2386,12 @@
         <v>11</v>
       </c>
       <c r="J48" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
@@ -2496,12 +2418,12 @@
         <v>11</v>
       </c>
       <c r="J49" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -2528,12 +2450,12 @@
         <v>11</v>
       </c>
       <c r="J50" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s">
         <v>11</v>
@@ -2560,12 +2482,12 @@
         <v>11</v>
       </c>
       <c r="J51" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
         <v>11</v>
@@ -2592,12 +2514,12 @@
         <v>11</v>
       </c>
       <c r="J52" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -2624,12 +2546,12 @@
         <v>11</v>
       </c>
       <c r="J53" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -2656,12 +2578,12 @@
         <v>11</v>
       </c>
       <c r="J54" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -2688,12 +2610,12 @@
         <v>11</v>
       </c>
       <c r="J55" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -2720,12 +2642,12 @@
         <v>11</v>
       </c>
       <c r="J56" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
@@ -2752,12 +2674,12 @@
         <v>11</v>
       </c>
       <c r="J57" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
@@ -2784,12 +2706,12 @@
         <v>11</v>
       </c>
       <c r="J58" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B59" t="s">
         <v>11</v>
@@ -2816,12 +2738,12 @@
         <v>11</v>
       </c>
       <c r="J59" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -2848,12 +2770,12 @@
         <v>11</v>
       </c>
       <c r="J60" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
@@ -2880,12 +2802,12 @@
         <v>11</v>
       </c>
       <c r="J61" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -2912,12 +2834,12 @@
         <v>11</v>
       </c>
       <c r="J62" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -2944,12 +2866,12 @@
         <v>11</v>
       </c>
       <c r="J63" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
@@ -2976,12 +2898,12 @@
         <v>11</v>
       </c>
       <c r="J64" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
@@ -3008,12 +2930,12 @@
         <v>11</v>
       </c>
       <c r="J65" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -3040,12 +2962,12 @@
         <v>11</v>
       </c>
       <c r="J66" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
@@ -3072,12 +2994,12 @@
         <v>11</v>
       </c>
       <c r="J67" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
@@ -3104,12 +3026,12 @@
         <v>11</v>
       </c>
       <c r="J68" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
         <v>11</v>
@@ -3136,12 +3058,12 @@
         <v>11</v>
       </c>
       <c r="J69" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
@@ -3168,12 +3090,12 @@
         <v>11</v>
       </c>
       <c r="J70" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B71" t="s">
         <v>11</v>
@@ -3200,12 +3122,12 @@
         <v>11</v>
       </c>
       <c r="J71" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B72" t="s">
         <v>11</v>
@@ -3232,12 +3154,12 @@
         <v>11</v>
       </c>
       <c r="J72" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
         <v>11</v>
@@ -3264,12 +3186,12 @@
         <v>11</v>
       </c>
       <c r="J73" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
@@ -3296,12 +3218,12 @@
         <v>11</v>
       </c>
       <c r="J74" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
@@ -3328,12 +3250,12 @@
         <v>11</v>
       </c>
       <c r="J75" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B76" t="s">
         <v>11</v>
@@ -3360,12 +3282,12 @@
         <v>11</v>
       </c>
       <c r="J76" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B77" t="s">
         <v>11</v>
@@ -3392,12 +3314,12 @@
         <v>11</v>
       </c>
       <c r="J77" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -3424,391 +3346,7 @@
         <v>11</v>
       </c>
       <c r="J78" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>152</v>
-      </c>
-      <c r="B79" t="s">
-        <v>11</v>
-      </c>
-      <c r="C79" t="s">
-        <v>11</v>
-      </c>
-      <c r="D79" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" t="s">
-        <v>11</v>
-      </c>
-      <c r="H79" t="s">
-        <v>11</v>
-      </c>
-      <c r="I79" t="s">
-        <v>11</v>
-      </c>
-      <c r="J79" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>152</v>
-      </c>
-      <c r="B80" t="s">
-        <v>11</v>
-      </c>
-      <c r="C80" t="s">
-        <v>11</v>
-      </c>
-      <c r="D80" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" t="s">
-        <v>11</v>
-      </c>
-      <c r="H80" t="s">
-        <v>11</v>
-      </c>
-      <c r="I80" t="s">
-        <v>11</v>
-      </c>
-      <c r="J80" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>152</v>
-      </c>
-      <c r="B81" t="s">
-        <v>11</v>
-      </c>
-      <c r="C81" t="s">
-        <v>11</v>
-      </c>
-      <c r="D81" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" t="s">
-        <v>11</v>
-      </c>
-      <c r="H81" t="s">
-        <v>11</v>
-      </c>
-      <c r="I81" t="s">
-        <v>11</v>
-      </c>
-      <c r="J81" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>156</v>
-      </c>
-      <c r="B82" t="s">
-        <v>11</v>
-      </c>
-      <c r="C82" t="s">
-        <v>11</v>
-      </c>
-      <c r="D82" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" t="s">
-        <v>11</v>
-      </c>
-      <c r="G82" t="s">
-        <v>11</v>
-      </c>
-      <c r="H82" t="s">
-        <v>11</v>
-      </c>
-      <c r="I82" t="s">
-        <v>11</v>
-      </c>
-      <c r="J82" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>158</v>
-      </c>
-      <c r="B83" t="s">
-        <v>11</v>
-      </c>
-      <c r="C83" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" t="s">
-        <v>11</v>
-      </c>
-      <c r="G83" t="s">
-        <v>11</v>
-      </c>
-      <c r="H83" t="s">
-        <v>11</v>
-      </c>
-      <c r="I83" t="s">
-        <v>11</v>
-      </c>
-      <c r="J83" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>160</v>
-      </c>
-      <c r="B84" t="s">
-        <v>11</v>
-      </c>
-      <c r="C84" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" t="s">
-        <v>11</v>
-      </c>
-      <c r="H84" t="s">
-        <v>11</v>
-      </c>
-      <c r="I84" t="s">
-        <v>11</v>
-      </c>
-      <c r="J84" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>162</v>
-      </c>
-      <c r="B85" t="s">
-        <v>11</v>
-      </c>
-      <c r="C85" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" t="s">
-        <v>11</v>
-      </c>
-      <c r="H85" t="s">
-        <v>11</v>
-      </c>
-      <c r="I85" t="s">
-        <v>11</v>
-      </c>
-      <c r="J85" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>164</v>
-      </c>
-      <c r="B86" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" t="s">
-        <v>11</v>
-      </c>
-      <c r="D86" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" t="s">
-        <v>11</v>
-      </c>
-      <c r="H86" t="s">
-        <v>11</v>
-      </c>
-      <c r="I86" t="s">
-        <v>11</v>
-      </c>
-      <c r="J86" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>164</v>
-      </c>
-      <c r="B87" t="s">
-        <v>11</v>
-      </c>
-      <c r="C87" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87" t="s">
-        <v>11</v>
-      </c>
-      <c r="H87" t="s">
-        <v>11</v>
-      </c>
-      <c r="I87" t="s">
-        <v>11</v>
-      </c>
-      <c r="J87" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>167</v>
-      </c>
-      <c r="B88" t="s">
-        <v>11</v>
-      </c>
-      <c r="C88" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" t="s">
-        <v>11</v>
-      </c>
-      <c r="G88" t="s">
-        <v>11</v>
-      </c>
-      <c r="H88" t="s">
-        <v>11</v>
-      </c>
-      <c r="I88" t="s">
-        <v>11</v>
-      </c>
-      <c r="J88" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>167</v>
-      </c>
-      <c r="B89" t="s">
-        <v>11</v>
-      </c>
-      <c r="C89" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" t="s">
-        <v>11</v>
-      </c>
-      <c r="H89" t="s">
-        <v>11</v>
-      </c>
-      <c r="I89" t="s">
-        <v>11</v>
-      </c>
-      <c r="J89" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>167</v>
-      </c>
-      <c r="B90" t="s">
-        <v>11</v>
-      </c>
-      <c r="C90" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" t="s">
-        <v>11</v>
-      </c>
-      <c r="H90" t="s">
-        <v>11</v>
-      </c>
-      <c r="I90" t="s">
-        <v>11</v>
-      </c>
-      <c r="J90" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: enhance password security and forgot password flow
- Add security warning 'Please change your password after first login' to all email templates
- Enhance forgot password email template with better styling and security warnings
- Add password strength validation requiring 8+ chars, uppercase, lowercase, numbers, special chars
- Real-time password strength indicator in reset password form
- Add security reminder notice to login page
- Improve password reset success messaging
- Enhanced email templates for better user experience

Security Features:
- Strong password requirements enforced during reset
- Visual feedback for password strength
- Security warnings in emails and UI
- Comprehensive validation before password reset

User Experience:
- Clear security messaging throughout the flow
- Real-time validation feedback
- Professional email templates
- Consistent security reminders
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="49">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,61 +43,121 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T13:23:23.245Z</t>
+    <t>2025-11-25T13:44:43.781Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"1157dfc2-7065-403f-b3fd-e5390a4de8ab","EventDtm":"2025-11-25T13:15:40Z","AppDtm":"2025-11-25T13:15:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:15:40Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":11,"GPSLastLock":6,"GPSLatitude":17.547901,"GPSLongitude":78.380641,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":33.5,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.270Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"41e1e6d5-48f2-49c2-984c-d82993454b6e","EventDtm":"2025-11-25T13:18:04Z","AppDtm":"2025-11-25T13:18:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:04Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.547749,"GPSLongitude":78.380502,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.271Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f82d6f34-15d4-48d9-9b29-50c2de392e91","EventDtm":"2025-11-25T13:18:12Z","AppDtm":"2025-11-25T13:18:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:12Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":16.891829,"GPSLongitude":79.475946,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:18:12Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":27.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":68.6,"TDisQ":null,"FreqComp":null,"TSuc":-32.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":39.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":8.84,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.286Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5dd699c5-479d-4e00-a646-05792c6f2265","EventDtm":"2025-11-25T13:18:40Z","AppDtm":"2025-11-25T13:18:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:40Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479477,"GPSLongitude":73.969695,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:18:40Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":26.75,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":140.13,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.72,"AmpPhB":10.06,"AmpPhC":10.72,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.93,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.7,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.55,"TRtn1Q":null,"TRtn2":5.56,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.4,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.291Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ac814ba2-ed0a-4eee-80c4-10a9f6532a9c","EventDtm":"2025-11-25T13:19:09Z","AppDtm":"2025-11-25T13:19:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:19:09Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.678724,"GPSLongitude":78.720129,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:19:09Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":24.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":140,"PSucQ":"asProvided","TDis":80.8,"TDisQ":null,"FreqComp":null,"TSuc":-4.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":950,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":504,"PctExpVlvQ":"OOR","TEvap":4.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":75.2,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":397,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":94.82,"PctSucVlvQ":null,"TSup1":3.81,"TSup1Q":null,"TSup2":3.7,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.297Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"27e9770d-dca4-42f7-8a3b-c97f028c17bb","EventDtm":"2025-11-25T13:19:35Z","AppDtm":"2025-11-25T13:19:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:19:35Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892069,"GPSLongitude":79.476266,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:19:35Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":73,"TDisQ":null,"FreqComp":null,"TSuc":-23.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":920,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":24,"PctExpVlvQ":null,"TEvap":-2.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.69,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":13.41,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.441Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7d536dca-189e-4da0-b698-bf7e8625141e","EventDtm":"2025-11-25T13:20:34Z","AppDtm":"2025-11-25T13:20:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:20:34Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533286,"GPSLongitude":78.433151,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:20:34Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":26.81,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":56.6,"TDisQ":null,"FreqComp":null,"TSuc":4,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":900,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":430.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"On","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.69,"TRtn1Q":null,"TRtn2":136.1,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":88.41,"PctSucVlvQ":null,"TSup1":3.12,"TSup1Q":null,"TSup2":3.3,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.448Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d3189edc-00c3-4efa-b8b6-736150a895bb","EventDtm":"2025-11-25T13:22:00Z","AppDtm":"2025-11-25T13:22:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:22:00Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.516187,"GPSLongitude":82.962413,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:22:00Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":25.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":84.3,"TDisQ":null,"FreqComp":null,"TSuc":-11,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":820,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":53,"PctExpVlvQ":null,"TEvap":22.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":389.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.5,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:23:23.450Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5c120761-ae95-4057-a5d9-95b272c685de","EventDtm":"2025-11-25T13:22:10Z","AppDtm":"2025-11-25T13:22:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:22:10Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310553,"GPSLongitude":91.717524,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:22:10Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":22.38,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":67.5,"TDisQ":null,"FreqComp":null,"TSuc":-28.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":70,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":84.15,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"41e1e6d5-48f2-49c2-984c-d82993454b6e","EventDtm":"2025-11-25T13:18:04Z","AppDtm":"2025-11-25T13:18:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:04Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.547749,"GPSLongitude":78.380502,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.817Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f82d6f34-15d4-48d9-9b29-50c2de392e91","EventDtm":"2025-11-25T13:18:12Z","AppDtm":"2025-11-25T13:18:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:12Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":16.891829,"GPSLongitude":79.475946,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:18:12Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":27.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":68.6,"TDisQ":null,"FreqComp":null,"TSuc":-32.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":39.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":8.84,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.824Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5dd699c5-479d-4e00-a646-05792c6f2265","EventDtm":"2025-11-25T13:18:40Z","AppDtm":"2025-11-25T13:18:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:40Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479477,"GPSLongitude":73.969695,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:18:40Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":26.75,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":140.13,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.72,"AmpPhB":10.06,"AmpPhC":10.72,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.93,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.7,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.55,"TRtn1Q":null,"TRtn2":5.56,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.4,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.828Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ac814ba2-ed0a-4eee-80c4-10a9f6532a9c","EventDtm":"2025-11-25T13:19:09Z","AppDtm":"2025-11-25T13:19:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:19:09Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.678724,"GPSLongitude":78.720129,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:19:09Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":24.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":140,"PSucQ":"asProvided","TDis":80.8,"TDisQ":null,"FreqComp":null,"TSuc":-4.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":950,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":504,"PctExpVlvQ":"OOR","TEvap":4.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":75.2,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":397,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":94.82,"PctSucVlvQ":null,"TSup1":3.81,"TSup1Q":null,"TSup2":3.7,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.976Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"27e9770d-dca4-42f7-8a3b-c97f028c17bb","EventDtm":"2025-11-25T13:19:35Z","AppDtm":"2025-11-25T13:19:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:19:35Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892069,"GPSLongitude":79.476266,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:19:35Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":73,"TDisQ":null,"FreqComp":null,"TSuc":-23.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":920,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":24,"PctExpVlvQ":null,"TEvap":-2.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.69,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":13.41,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.987Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7d536dca-189e-4da0-b698-bf7e8625141e","EventDtm":"2025-11-25T13:20:34Z","AppDtm":"2025-11-25T13:20:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:20:34Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533286,"GPSLongitude":78.433151,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:20:34Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":26.81,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":56.6,"TDisQ":null,"FreqComp":null,"TSuc":4,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":900,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":430.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"On","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.69,"TRtn1Q":null,"TRtn2":136.1,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":88.41,"PctSucVlvQ":null,"TSup1":3.12,"TSup1Q":null,"TSup2":3.3,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.992Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d3189edc-00c3-4efa-b8b6-736150a895bb","EventDtm":"2025-11-25T13:22:00Z","AppDtm":"2025-11-25T13:22:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:22:00Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.516187,"GPSLongitude":82.962413,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:22:00Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":25.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":84.3,"TDisQ":null,"FreqComp":null,"TSuc":-11,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":820,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":53,"PctExpVlvQ":null,"TEvap":22.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":389.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.5,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:43.996Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5c120761-ae95-4057-a5d9-95b272c685de","EventDtm":"2025-11-25T13:22:10Z","AppDtm":"2025-11-25T13:22:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:22:10Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310553,"GPSLongitude":91.717524,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:22:10Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":22.38,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":67.5,"TDisQ":null,"FreqComp":null,"TSuc":-28.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":70,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":84.15,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.002Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3bc5bc27-bad8-40fb-a914-cfa28f9e4ea5","EventDtm":"2025-11-25T13:23:42Z","AppDtm":"2025-11-25T13:23:56Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:23:42Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804937,"GPSLongitude":77.662302,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:23:42Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":93.48,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.44,"AmpPhB":11.19,"AmpPhC":11.44,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.69,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.82,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.74,"PctSucVlvQ":null,"TSup1":5.06,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.015Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8028bb08-a8ab-45e6-9f29-52e53c81893f","EventDtm":"2025-11-25T13:24:32Z","AppDtm":"2025-11-25T13:24:46Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:24:32Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":28.364765,"GPSLongitude":75.581265,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:24:32Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":16,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":33,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":5.3,"AmpPhB":6.3,"AmpPhC":6,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":404,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":5.8,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.025Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bd325df3-fe0a-4853-bec2-598af390d790","EventDtm":"2025-11-25T13:25:39Z","AppDtm":"2025-11-25T13:25:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:25:39Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.516074,"GPSLongitude":82.981253,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:25:39Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":27.05,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":145.79,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":10.74,"AmpPhB":10.89,"AmpPhC":10.74,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":3.63,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.11,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.65,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.02,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.61,"TRtn1Q":null,"TRtn2":3.65,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.25,"PctSucVlvQ":null,"TSup1":3.04,"TSup1Q":null,"TSup2":3.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.032Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"39ed703d-67b6-48a7-8da5-eac1ec017b41","EventDtm":"2025-11-25T15:09:15Z","AppDtm":"2025-11-25T13:27:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T15:09:15Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":4198,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.036Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5b5648a2-0ae0-4902-b0a7-4ac9a925829c","EventDtm":"2025-11-25T13:30:43Z","AppDtm":"2025-11-25T13:31:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:30:43Z","DeviceID":"JSGA623040314","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":2,"GPSLatitude":19.252887,"GPSLongitude":73.016518,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:30:43Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":28.96,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.55,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.85,"AmpPhB":11.34,"AmpPhC":10.85,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.81,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":404.81,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.12,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.33,"TRtn1Q":null,"TRtn2":5.46,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":3.11,"PctSucVlvQ":null,"TSup1":7.91,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.039Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0fb213d9-1e38-4857-8461-9419fdc0f428","EventDtm":"2025-11-25T13:30:50Z","AppDtm":"2025-11-25T13:31:06Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:30:50Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":28.678867,"GPSLongitude":77.599718,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:30:50Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":20.16,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":60.64,"PSucQ":null,"TDis":40.39,"TDisQ":null,"FreqComp":null,"TSuc":18.81,"TSucQ":null,"MCond":0,"PCond":270.28,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04475864","AmpPhA":0,"AmpPhB":0.01,"AmpPhC":0,"PDis":88.72,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":19.4,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":67.73,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.78,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":19.84,"TRtn1Q":null,"TRtn2":19.82,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":18.87,"TSup1Q":null,"TSup2":18.75,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.041Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a2c58028-5e3d-4669-a9f7-fcf68d0a774b","EventDtm":"2025-11-25T13:33:39Z","AppDtm":"2025-11-25T13:33:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:33:39Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804954,"GPSLongitude":77.662305,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:33:39Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.93,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":96.36,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.48,"AmpPhB":11.1,"AmpPhC":11.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.38,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.03,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.043Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bdc11915-8fff-4b61-8348-7abdb8a12b0f","EventDtm":"2025-11-25T13:35:36Z","AppDtm":"2025-11-25T13:35:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:35:36Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.657916,"GPSLongitude":83.101703,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":7.9,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:35:36Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":27.34,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":67.16,"PSucQ":null,"TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":119.64,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.93,"AmpPhB":1.58,"AmpPhC":0.93,"PDis":134.85,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.49,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.85,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.22,"TRtn1Q":null,"TRtn2":20.24,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":20.52,"PctSucVlvQ":null,"TSup1":19.53,"TSup1Q":null,"TSup2":19.59,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.045Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"55d9ed19-30ac-4fce-92dc-0f06264186c7","EventDtm":"2025-11-25T13:35:51Z","AppDtm":"2025-11-25T13:36:08Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:35:51Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.892056,"GPSLongitude":79.476138,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:35:51Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":27.35,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":150.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":10.56,"AmpPhB":10.38,"AmpPhC":10.56,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.2,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.75,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.79,"TRtn1Q":null,"TRtn2":17.73,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.12,"PctSucVlvQ":null,"TSup1":18.55,"TSup1Q":null,"TSup2":18.58,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.172Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3bbed495-def7-41cb-933e-d31f3303fc21","EventDtm":"2025-11-25T13:35:56Z","AppDtm":"2025-11-25T13:36:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:35:56Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.805015,"GPSLongitude":77.662236,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:35:56Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":23,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":94.24,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.85,"AmpPhB":10.65,"AmpPhC":10.85,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.94,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.38,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.88,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.33,"TRtn1Q":null,"TRtn2":5.33,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":2.59,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T13:44:44.187Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"94a6ba65-f6c2-4fbc-9773-39137ea671f3","EventDtm":"2025-11-25T13:41:43Z","AppDtm":"2025-11-25T13:42:01Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:41:43Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.57235,"GPSLongitude":78.515101,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323415","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
   </si>
 </sst>
 </file>
@@ -486,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -825,6 +885,326 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
fix: add missing DialogDescription imports to prevent blank pages
- Added DialogDescription import to client-profile.tsx
- Added DialogDescription and DialogFooter imports to technician-profile.tsx
- Fixed JavaScript ReferenceError that was causing pages to render blank
- Confirmation dialogs for Send Credentials now work properly

Root Cause: When adding confirmation dialogs, DialogDescription component
was used but not imported, causing runtime JavaScript errors that prevented
page rendering entirely.
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="71">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,121 +43,187 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T13:44:43.781Z</t>
+    <t>2025-11-25T14:18:39.501Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"41e1e6d5-48f2-49c2-984c-d82993454b6e","EventDtm":"2025-11-25T13:18:04Z","AppDtm":"2025-11-25T13:18:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:04Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.547749,"GPSLongitude":78.380502,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.817Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"f82d6f34-15d4-48d9-9b29-50c2de392e91","EventDtm":"2025-11-25T13:18:12Z","AppDtm":"2025-11-25T13:18:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:12Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":16.891829,"GPSLongitude":79.475946,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:18:12Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":27.38,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":68.6,"TDisQ":null,"FreqComp":null,"TSuc":-32.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":39.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":8.84,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":12,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.824Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5dd699c5-479d-4e00-a646-05792c6f2265","EventDtm":"2025-11-25T13:18:40Z","AppDtm":"2025-11-25T13:18:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:18:40Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479477,"GPSLongitude":73.969695,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:18:40Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":26.75,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":140.13,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.72,"AmpPhB":10.06,"AmpPhC":10.72,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.93,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":88.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.7,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.55,"TRtn1Q":null,"TRtn2":5.56,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.4,"PctSucVlvQ":null,"TSup1":4.94,"TSup1Q":null,"TSup2":4.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.828Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ac814ba2-ed0a-4eee-80c4-10a9f6532a9c","EventDtm":"2025-11-25T13:19:09Z","AppDtm":"2025-11-25T13:19:25Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:19:09Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.678724,"GPSLongitude":78.720129,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:19:09Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":24.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":140,"PSucQ":"asProvided","TDis":80.8,"TDisQ":null,"FreqComp":null,"TSuc":-4.1,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":950,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":504,"PctExpVlvQ":"OOR","TEvap":4.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":75.2,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":397,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.12,"TRtn1Q":null,"TRtn2":6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":94.82,"PctSucVlvQ":null,"TSup1":3.81,"TSup1Q":null,"TSup2":3.7,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.976Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"27e9770d-dca4-42f7-8a3b-c97f028c17bb","EventDtm":"2025-11-25T13:19:35Z","AppDtm":"2025-11-25T13:19:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:19:35Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.892069,"GPSLongitude":79.476266,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:19:35Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":27.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":0,"PSucQ":"asProvided","TDis":73,"TDisQ":null,"FreqComp":null,"TSuc":-23.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":920,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":24,"PctExpVlvQ":null,"TEvap":-2.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.69,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":13.41,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.987Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7d536dca-189e-4da0-b698-bf7e8625141e","EventDtm":"2025-11-25T13:20:34Z","AppDtm":"2025-11-25T13:20:54Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:20:34Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533286,"GPSLongitude":78.433151,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:20:34Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":26.81,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":56.6,"TDisQ":null,"FreqComp":null,"TSuc":4,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":900,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":430.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"On","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.69,"TRtn1Q":null,"TRtn2":136.1,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":88.41,"PctSucVlvQ":null,"TSup1":3.12,"TSup1Q":null,"TSup2":3.3,"TSup2Q":null,"AmpTotalDraw":0,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.992Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d3189edc-00c3-4efa-b8b6-736150a895bb","EventDtm":"2025-11-25T13:22:00Z","AppDtm":"2025-11-25T13:22:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:22:00Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.516187,"GPSLongitude":82.962413,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.2,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:22:00Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":25.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":84.3,"TDisQ":null,"FreqComp":null,"TSuc":-11,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":820,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":53,"PctExpVlvQ":null,"TEvap":22.12,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":389.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.5,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:43.996Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5c120761-ae95-4057-a5d9-95b272c685de","EventDtm":"2025-11-25T13:22:10Z","AppDtm":"2025-11-25T13:22:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:22:10Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310553,"GPSLongitude":91.717524,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:22:10Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":22.38,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":67.5,"TDisQ":null,"FreqComp":null,"TSuc":-28.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":70,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":84.15,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.8,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.002Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3bc5bc27-bad8-40fb-a914-cfa28f9e4ea5","EventDtm":"2025-11-25T13:23:42Z","AppDtm":"2025-11-25T13:23:56Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:23:42Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804937,"GPSLongitude":77.662302,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:23:42Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.67,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":93.48,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.44,"AmpPhB":11.19,"AmpPhC":11.44,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.69,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.81,"TRtn1Q":null,"TRtn2":5.82,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.74,"PctSucVlvQ":null,"TSup1":5.06,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.015Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8028bb08-a8ab-45e6-9f29-52e53c81893f","EventDtm":"2025-11-25T13:24:32Z","AppDtm":"2025-11-25T13:24:46Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:24:32Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":28.364765,"GPSLongitude":75.581265,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:24:32Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":16,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":33,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":5.3,"AmpPhB":6.3,"AmpPhC":6,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":17,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":404,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":5.8,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.025Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bd325df3-fe0a-4853-bec2-598af390d790","EventDtm":"2025-11-25T13:25:39Z","AppDtm":"2025-11-25T13:25:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:25:39Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.516074,"GPSLongitude":82.981253,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:25:39Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":27.05,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":145.79,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":10.74,"AmpPhB":10.89,"AmpPhC":10.74,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":3.63,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.11,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.65,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.02,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.61,"TRtn1Q":null,"TRtn2":3.65,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.25,"PctSucVlvQ":null,"TSup1":3.04,"TSup1Q":null,"TSup2":3.04,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.032Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"39ed703d-67b6-48a7-8da5-eac1ec017b41","EventDtm":"2025-11-25T15:09:15Z","AppDtm":"2025-11-25T13:27:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T15:09:15Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":4198,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-77","ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.036Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5b5648a2-0ae0-4902-b0a7-4ac9a925829c","EventDtm":"2025-11-25T13:30:43Z","AppDtm":"2025-11-25T13:31:03Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:30:43Z","DeviceID":"JSGA623040314","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":2,"GPSLatitude":19.252887,"GPSLongitude":73.016518,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578863","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1036859","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:30:43Z","AssetType":"Reefer","AssetID":"CCLU1036859","OEM":"CARRIER","TAmb":28.96,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":3,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-189.06,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.55,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04547502","AmpPhA":10.85,"AmpPhB":11.34,"AmpPhC":10.85,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.81,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":404.81,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.12,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.33,"TRtn1Q":null,"TRtn2":5.46,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5186","VerSWMinor":null,"PctSucVlv":3.11,"PctSucVlvQ":null,"TSup1":7.91,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-11T12:04:15Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.039Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0fb213d9-1e38-4857-8461-9419fdc0f428","EventDtm":"2025-11-25T13:30:50Z","AppDtm":"2025-11-25T13:31:06Z","Events":["ACPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:30:50Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":28.678867,"GPSLongitude":77.599718,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":29.2,"BatteryVoltage":8,"DeviceTemp":23,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:30:50Z","AssetType":"Reefer","AssetID":"SJKU4000017","OEM":"CARRIER","TAmb":20.16,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":60.64,"PSucQ":null,"TDis":40.39,"TDisQ":null,"FreqComp":null,"TSuc":18.81,"TSucQ":null,"MCond":0,"PCond":270.28,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04475864","AmpPhA":0,"AmpPhB":0.01,"AmpPhC":0,"PDis":88.72,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":19.4,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":67.73,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":413.78,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":19.84,"TRtn1Q":null,"TRtn2":19.82,"TRtn2Q":null,"TSet":17.2,"TSetQ":null,"VerSWMajor":"5370","VerSWMinor":null,"PctSucVlv":10,"PctSucVlvQ":null,"TSup1":18.87,"TSup1Q":null,"TSup2":18.75,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-23T08:47:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.041Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a2c58028-5e3d-4669-a9f7-fcf68d0a774b","EventDtm":"2025-11-25T13:33:39Z","AppDtm":"2025-11-25T13:33:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:33:39Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804954,"GPSLongitude":77.662305,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:33:39Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.93,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":96.36,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.48,"AmpPhB":11.1,"AmpPhC":11.48,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.21,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":415.38,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.03,"PctSucVlvQ":null,"TSup1":4.96,"TSup1Q":null,"TSup2":4.89,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.043Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bdc11915-8fff-4b61-8348-7abdb8a12b0f","EventDtm":"2025-11-25T13:35:36Z","AppDtm":"2025-11-25T13:35:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:35:36Z","DeviceID":"JSGA623040320","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.657916,"GPSLongitude":83.101703,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232723478","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":7.9,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6712079","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:35:36Z","AssetType":"Reefer","AssetID":"KKFU6712079","OEM":"CARRIER","TAmb":27.34,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":0,"PctCO2SetQ":null,"PSuc":67.16,"PSucQ":null,"TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":119.64,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04742313","AmpPhA":0.93,"AmpPhB":1.58,"AmpPhC":0.93,"PDis":134.85,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":20.49,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.85,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":0,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":20.22,"TRtn1Q":null,"TRtn2":20.24,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5154","VerSWMinor":null,"PctSucVlv":20.52,"PctSucVlvQ":null,"TSup1":19.53,"TSup1Q":null,"TSup2":19.59,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-03-28T10:32:52Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.045Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"55d9ed19-30ac-4fce-92dc-0f06264186c7","EventDtm":"2025-11-25T13:35:51Z","AppDtm":"2025-11-25T13:36:08Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:35:51Z","DeviceID":"JSGA623040187","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":16.892056,"GPSLongitude":79.476138,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-63","ExtPower":true,"ExtPowerVoltage":30.2,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"GSOU6384153","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:35:51Z","AssetType":"Reefer","AssetID":"GSOU6384153","OEM":"CARRIER","TAmb":27.35,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-190.62,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":150.21,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04251422","AmpPhA":10.56,"AmpPhB":10.38,"AmpPhC":10.56,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":18.1,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":92.2,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":410.75,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":17.79,"TRtn1Q":null,"TRtn2":17.73,"TRtn2Q":null,"TSet":18.5,"TSetQ":null,"VerSWMajor":"5167","VerSWMinor":null,"PctSucVlv":2.12,"PctSucVlvQ":null,"TSup1":18.55,"TSup1Q":null,"TSup2":18.58,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-04T10:10:59Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.172Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3bbed495-def7-41cb-933e-d31f3303fc21","EventDtm":"2025-11-25T13:35:56Z","AppDtm":"2025-11-25T13:36:11Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:35:56Z","DeviceID":"JSGA623040262","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":12.805015,"GPSLongitude":77.662236,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.7,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681542","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:35:56Z","AssetType":"Reefer","AssetID":"TRIU6681542","OEM":"CARRIER","TAmb":23,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":94.24,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04958167","AmpPhA":10.85,"AmpPhB":10.65,"AmpPhC":10.85,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.94,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.38,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.88,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.33,"TRtn1Q":null,"TRtn2":5.33,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":2.59,"PctSucVlvQ":null,"TSup1":5.01,"TSup1Q":null,"TSup2":5.01,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T09:58:17Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T13:44:44.187Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"94a6ba65-f6c2-4fbc-9773-39137ea671f3","EventDtm":"2025-11-25T13:41:43Z","AppDtm":"2025-11-25T13:42:01Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:41:43Z","DeviceID":"JSGA623040277","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.57235,"GPSLongitude":78.515101,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19327","CID":"235323415","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"DFOU6120281","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"299528ec-592f-461a-9149-a5a0e8546610","EventDtm":"2025-11-25T13:43:39Z","AppDtm":"2025-11-25T13:43:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:43:39Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":12.804993,"GPSLongitude":77.66229,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904096","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.6,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:43:39Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.64,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":92.24,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.62,"AmpPhB":11.23,"AmpPhC":11.62,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.18,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":419.07,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.01,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.73,"TRtn1Q":null,"TRtn2":5.75,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.46,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.663Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"b39054dd-b3b0-4b04-a7fe-285a1e4ba763","EventDtm":"2025-11-25T13:43:57Z","AppDtm":"2025-11-25T13:44:14Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:43:57Z","DeviceID":"JSGA623040298","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.657964,"GPSLongitude":83.101733,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"233290773","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"KKFU6994964","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:43:57Z","AssetType":"Reefer","AssetID":"KKFU6994964","OEM":"CARRIER","TAmb":27.25,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":71.73,"PSucQ":null,"TDis":-189.84,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":0,"PCond":102.78,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Idle","SnCtrl":"04783085","AmpPhA":0.93,"AmpPhB":1.55,"AmpPhC":0.93,"PDis":102.55,"PDisQ":null,"PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":21.24,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0.04,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":421.41,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":20.87,"TRtn1Q":null,"TRtn2":20.93,"TRtn2Q":null,"TSet":20,"TSetQ":null,"VerSWMajor":"5156","VerSWMinor":null,"PctSucVlv":20.6,"PctSucVlvQ":null,"TSup1":21.22,"TSup1Q":null,"TSup2":21.29,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-11-29T10:30:33Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.694Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"0a12b727-3eb6-454d-884a-8d2d9ff431d0","EventDtm":"2025-11-25T13:50:05Z","AppDtm":"2025-11-25T13:50:19Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:50:05Z","DeviceID":"JSGA623040284","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.537141,"GPSLongitude":78.175613,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"247361559","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6618637","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:50:05Z","AssetType":"Reefer","AssetID":"TRIU6618637","OEM":"CARRIER","TAmb":25.88,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":0,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":135.48,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04898885","AmpPhA":11.19,"AmpPhB":11.62,"AmpPhC":11.19,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":-23.26,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":0,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":16.06,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414.88,"VLine2":null,"VLine3":null,"MEvapFanLS":1,"PctO2":0,"PctO2Q":"asProvided","PctO2Set":10,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":-17.33,"TRtn1Q":null,"TRtn2":-17.37,"TRtn2Q":null,"TSet":-20,"TSetQ":null,"VerSWMajor":"5168","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":-31.92,"TSup1Q":null,"TSup2":-31.12,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T10:27:06Z","PTIResult":"Skipped","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":52,"RCAlias":"AL52","RCSeverity":"Minor","Active":true},{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.713Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4ec4a542-7aed-4e47-98b4-0925b6855554","EventDtm":"2025-11-25T13:51:30Z","AppDtm":"2025-11-25T13:51:45Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:51:30Z","DeviceID":"JSGA623040278","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":17.532982,"GPSLongitude":78.433498,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"230743318","RSSI":"-57","ExtPower":true,"ExtPowerVoltage":33.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1026520","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:51:30Z","AssetType":"Reefer","AssetID":"CXRU1026520","OEM":"DAIKIN","TAmb":25.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":72.6,"TDisQ":null,"FreqComp":null,"TSuc":-28.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":810,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.31,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":95,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":422.1,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":6.31,"TRtn1Q":null,"TRtn2":6.4,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.37,"PctSucVlvQ":null,"TSup1":5.19,"TSup1Q":null,"TSup2":5.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-31T08:13:55Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.729Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"203660e5-7dbc-4cd3-9688-a2e4750367e5","EventDtm":"2025-11-25T13:51:49Z","AppDtm":"2025-11-25T13:52:05Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:51:49Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.678684,"GPSLongitude":78.720176,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.2,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:51:49Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":24.19,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":220,"PSucQ":"asProvided","TDis":89.7,"TDisQ":null,"FreqComp":null,"TSuc":4.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":650,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":800,"PctExpVlvQ":"OOR","TEvap":2.69,"TEvapQ":null,"MCtrl3":"PTIEmergencyStop1","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":90.16,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":395.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.19,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":12.2,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":107,"RCAlias":"E107","RCSeverity":"Severe","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.772Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6f29dc51-b6ad-4e15-a5aa-3592945894b6","EventDtm":"2025-11-25T13:53:45Z","AppDtm":"2025-11-25T13:53:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:53:45Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804997,"GPSLongitude":77.662208,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:53:45Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.57,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":93.35,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.5,"AmpPhB":11.26,"AmpPhC":11.5,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.22,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":418.18,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.79,"TRtn1Q":null,"TRtn2":5.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.44,"PctSucVlvQ":null,"TSup1":5.06,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.795Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":7,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"189527fc-f89d-460a-b4f1-72a65df0f5b8","EventDtm":"2025-11-25T13:55:22Z","AppDtm":"2025-11-25T13:55:35Z","Events":["MicroAlarm"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:55:22Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.678717,"GPSLongitude":78.720193,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.4,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:55:22Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":23.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":70,"PSucQ":"asProvided","TDis":53.2,"TDisQ":null,"FreqComp":null,"TSuc":13.6,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":820,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":400,"PctExpVlvQ":"OOR","TEvap":4,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"Off","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":90.16,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":397.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.19,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":100,"PctSucVlvQ":null,"TSup1":4.38,"TSup1Q":null,"TSup2":4.4,"TSup2Q":null,"AmpTotalDraw":1,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.817Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":8,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9237d526-f0a7-49e4-8933-69528b7c5ee4","EventDtm":"2025-11-25T13:55:35Z","AppDtm":"2025-11-25T13:55:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:55:35Z","DeviceID":"JSGA623040182","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.538932,"GPSLongitude":78.178275,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19397","CID":"232155661","RSSI":"-55","ExtPower":true,"ExtPowerVoltage":32.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU5800414","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T13:55:35Z","AssetType":"Reefer","AssetID":"TDRU5800414","OEM":"DAIKIN","TAmb":25.19,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-50,"PSucQ":"asProvided","TDis":112.7,"TDisQ":null,"FreqComp":null,"TSuc":-36.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":20,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":98.82,"PctHumQ":null,"PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":412.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5,"TRtn1Q":null,"TRtn2":4.9,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":82.32,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.4,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-30T07:54:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.841Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":9,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"5fbf4d7c-680b-49d5-8d9e-d3f34e51abe9","EventDtm":"2025-11-25T13:58:09Z","AppDtm":"2025-11-25T13:58:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T13:58:09Z","DeviceID":"JSGA623040311","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":26.606064,"GPSLongitude":80.723776,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"15","LAC":"55363","CID":"210193709","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.8,"BatteryVoltage":8,"DeviceTemp":19,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.862Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":10,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4d8ccaf7-1030-466e-9329-d04012e7646e","EventDtm":"2025-11-25T14:01:04Z","AppDtm":"2025-11-25T14:01:23Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:01:04Z","DeviceID":"JSGA623040164","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":21.735615,"GPSLongitude":72.628795,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"98","LAC":"8405","CID":"246992643","RSSI":"-69","ExtPower":true,"ExtPowerVoltage":31,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1031878","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:01:04Z","AssetType":"Reefer","AssetID":"CCLU1031878","OEM":"CARRIER","TAmb":30.19,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":15,"PctCO2Q":null,"PctCO2Set":5,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":161.74,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04502009","AmpPhA":13.6,"AmpPhB":13.12,"AmpPhC":13.6,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":16.16,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":90.79,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":435.25,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.08,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":15.45,"TRtn1Q":null,"TRtn2":15.41,"TRtn2Q":null,"TSet":15,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":2.21,"PctSucVlvQ":null,"TSup1":15.11,"TSup1Q":null,"TSup2":15.28,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-03-09T09:34:16Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.894Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":11,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"67a669d0-51e5-4387-8b91-9fe87f4a606e","EventDtm":"2025-11-25T14:02:00Z","AppDtm":"2025-11-25T14:02:18Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:02:00Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":26.644437,"GPSLongitude":88.468006,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.5,"BatteryVoltage":8.1,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:02:00Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":22,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":85.7,"TDisQ":null,"FreqComp":null,"TSuc":-30.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":-0.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":416.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":0.81,"TRtn1Q":null,"TRtn2":1.6,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":0.12,"TSup1Q":null,"TSup2":1.8,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.902Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":12,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"4ea524bb-f70e-4d42-ad88-006413840fe8","EventDtm":"2025-11-25T14:02:57Z","AppDtm":"2025-11-25T14:03:12Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:02:57Z","DeviceID":"JSGA621320194","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":16.824876,"GPSLongitude":78.131542,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31204","CID":"255654657","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.1,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1186425","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:02:57Z","AssetType":"Reefer","AssetID":"CXRU1186425","OEM":"DAIKIN","TAmb":26.5,"TAmbQ":null,"TUSDA4":-46.5,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":64.4,"TDisQ":null,"FreqComp":null,"TSuc":-26.2,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":910,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":37,"PctExpVlvQ":null,"TEvap":9.88,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":405.7,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.88,"TRtn1Q":null,"TRtn2":4.8,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":5,"TSup1Q":null,"TSup2":5.5,"TSup2Q":null,"AmpTotalDraw":17,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.5,"TUSDA1Q":"OOR","TUSDA2":-46.5,"TUSDA2Q":"OOR","TUSDA3":-46.5,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-06-30T05:28:13Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.919Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":13,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"808589f8-bc49-4d1a-b4ab-0076da1b7c0f","EventDtm":"2025-11-25T14:03:44Z","AppDtm":"2025-11-25T14:03:57Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:03:44Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":12.804982,"GPSLongitude":77.662226,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:03:44Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.66,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":98.53,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.76,"AmpPhB":11.3,"AmpPhC":11.76,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.2,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":417.79,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.03,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.76,"TRtn1Q":null,"TRtn2":5.79,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.99,"PctSucVlvQ":null,"TSup1":4.98,"TSup1Q":null,"TSup2":4.91,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.930Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":14,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"15aa3d9e-e5b0-4c42-bd21-cf870ff11991","EventDtm":"2025-11-25T14:06:41Z","AppDtm":"2025-11-25T14:06:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:06:41Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.67908,"GPSLongitude":78.720148,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":27,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:06:41Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":23.75,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-183.2,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":130.33,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":10.84,"AmpPhB":10.31,"AmpPhC":10.84,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.33,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":405.45,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.11,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.83,"TRtn1Q":null,"TRtn2":4.83,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":5.31,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4.16,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.944Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":15,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"7e353359-fc83-4ddd-a690-eb280d1672d5","EventDtm":"2025-11-25T14:07:24Z","AppDtm":"2025-11-25T14:07:44Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:07:24Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678913,"GPSLongitude":77.59986,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"128143137","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":7.8,"BatteryVoltage":8,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.953Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":16,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a6d87e9e-8881-4889-bd1a-5ddd54c8e02c","EventDtm":"2025-11-25T14:09:14Z","AppDtm":"2025-11-25T14:09:32Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:09:14Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.661631,"GPSLongitude":83.089137,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.6,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:09:14Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":29.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":40,"PSucQ":"asProvided","TDis":44.7,"TDisQ":null,"FreqComp":null,"TSuc":-14.7,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1020,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":371.4,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.2,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":96.04,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.8,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.980Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":17,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"9386ca31-7774-4f79-8fab-40859112a403","EventDtm":"2025-11-25T14:13:40Z","AppDtm":"2025-11-25T14:13:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:13:40Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":12.804973,"GPSLongitude":77.662183,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":29,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:13:40Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.37,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":93.39,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.37,"AmpPhB":11.02,"AmpPhC":11.37,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.17,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":414,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.07,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.74,"TRtn1Q":null,"TRtn2":5.76,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":4.2,"PctSucVlvQ":null,"TSup1":4.93,"TSup1Q":null,"TSup2":4.86,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.984Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":18,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"772cd31b-e3c4-4bdc-96c9-7712f4918a44","EventDtm":"2025-11-25T14:14:30Z","AppDtm":"2025-11-25T14:14:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:14:30Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":12,"GPSLastLock":0,"GPSLatitude":19.252936,"GPSLongitude":73.016506,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30.4,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.988Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":19,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"332e03ca-c427-499a-b888-280c27f7f1d7","EventDtm":"2025-11-25T14:16:02Z","AppDtm":"2025-11-25T14:16:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:16:02Z","DeviceID":"JSGA623040329","GPSLockState":"LOCKED","GPSSatelliteCount":11,"GPSLastLock":0,"GPSLatitude":17.547952,"GPSLongitude":78.380584,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":33.9,"BatteryVoltage":8,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:39.993Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":20,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"939c2962-5380-4b75-b124-998f43b8afff","EventDtm":"2025-11-25T14:18:19Z","AppDtm":"2025-11-25T14:18:34Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:18:19Z","DeviceID":"JSGA622180052","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.547767,"GPSLongitude":78.380492,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34.2,"BatteryVoltage":8.1,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:40.002Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":21,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3d935570-8138-4448-aeaa-ad72145d5a0e","EventDtm":"2025-11-25T14:18:19Z","AppDtm":"2025-11-25T14:18:36Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:18:19Z","DeviceID":"JSGA622340187","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":16.891835,"GPSLongitude":79.476016,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-75","ExtPower":true,"ExtPowerVoltage":32.9,"BatteryVoltage":8,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1032564","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:18:19Z","AssetType":"Reefer","AssetID":"CXRU1032564","OEM":"DAIKIN","TAmb":26.5,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-40,"PSucQ":"asProvided","TDis":67.3,"TDisQ":null,"FreqComp":null,"TSuc":-32.5,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":820,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":14,"PctExpVlvQ":null,"TEvap":3.62,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":411.6,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.31,"TRtn1Q":null,"TRtn2":39.6,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":8.84,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T06:44:58Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:18:50.766Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":22,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6bccca7e-0980-43dc-976a-4b3ee0425adb","EventDtm":"2025-11-25T14:18:37Z","AppDtm":"2025-11-25T14:18:50Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:18:37Z","DeviceID":"JSGA623040304","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":15.479508,"GPSLongitude":73.969701,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6934","CID":"242082151","RSSI":"-71","ExtPower":true,"ExtPowerVoltage":29.5,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681434","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:18:37Z","AssetType":"Reefer","AssetID":"TRIU6681434","OEM":"CARRIER","TAmb":26.05,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":140.48,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04959272","AmpPhA":10.96,"AmpPhB":10.48,"AmpPhC":10.96,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.92,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":87.64,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":423.46,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.09,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.53,"TRtn1Q":null,"TRtn2":5.55,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.51,"PctSucVlvQ":null,"TSup1":4.91,"TSup1Q":null,"TSup2":4.93,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-08-19T12:53:23Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:19:24.686Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":23,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"d366f263-36c5-4d1f-8cc9-692201738281","EventDtm":"2025-11-25T14:19:09Z","AppDtm":"2025-11-25T14:19:24Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:19:09Z","DeviceID":"JSGA622340482","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":17.678744,"GPSLongitude":78.720189,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963203","RSSI":null,"ExtPower":true,"ExtPowerVoltage":31.3,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CAIU5422720","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:19:09Z","AssetType":"Reefer","AssetID":"CAIU5422720","OEM":"DAIKIN","TAmb":24.12,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":90.7,"TDisQ":null,"FreqComp":null,"TSuc":1.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":770,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":700,"PctExpVlvQ":"OOR","TEvap":2.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":90.94,"PctHumQ":null,"PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":392.2,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.88,"TRtn1Q":null,"TRtn2":4.8,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"27C2","VerSWMinor":null,"PctSucVlv":10.67,"PctSucVlvQ":null,"TSup1":4,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-10-30T05:56:46Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:19:52.239Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":24,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"bf4d8462-158a-4128-94a1-b8e2fdfc3e56","EventDtm":"2025-11-25T14:19:33Z","AppDtm":"2025-11-25T14:19:52Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:19:33Z","DeviceID":"JSGA623040309","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":16.892106,"GPSLongitude":79.476194,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31802","CID":"247193878","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":31.9,"BatteryVoltage":8,"DeviceTemp":31,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1045896","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:19:33Z","AssetType":"Reefer","AssetID":"CXRU1045896","OEM":"DAIKIN","TAmb":26.31,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-30,"PSucQ":"asProvided","TDis":77.9,"TDisQ":null,"FreqComp":null,"TSuc":-28.4,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":780,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":16,"PctExpVlvQ":null,"TEvap":-1.81,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":409,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":4.38,"TRtn1Q":null,"TRtn2":5,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.98,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":4,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-04T07:47:44Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:20:47.709Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":25,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"ec1d457f-84b1-4be2-b2fc-1de6a9582a8e","EventDtm":"2025-11-25T14:20:32Z","AppDtm":"2025-11-25T14:20:47Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:20:32Z","DeviceID":"JSGA623040188","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.533195,"GPSLongitude":78.433093,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19315","CID":"244342551","RSSI":null,"ExtPower":true,"ExtPowerVoltage":33.5,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"HDMU5221979","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:20:32Z","AssetType":"Reefer","AssetID":"HDMU5221979","OEM":"DAIKIN","TAmb":26.19,"TAmbQ":null,"TUSDA4":-46.3,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":240,"PSucQ":"asProvided","TDis":49.9,"TDisQ":null,"FreqComp":null,"TSuc":5.6,"TSucQ":null,"MCond":"Off","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":860,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":5,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"ThermoOff","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":14.96,"PctHumQ":null,"PctHumSet":65,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":426.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"FanReduction","TRtn1":5.69,"TRtn1Q":null,"TRtn2":136.1,"TRtn2Q":"OOR","TSet":5,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":85.06,"PctSucVlvQ":null,"TSup1":4.69,"TSup1Q":null,"TSup2":4.8,"TSup2Q":null,"AmpTotalDraw":2,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.3,"TUSDA1Q":"OOR","TUSDA2":-46.2,"TUSDA2Q":"OOR","TUSDA3":-46.3,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-02-13T11:13:57Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true},{"OemAlarm":404,"RCAlias":"E404","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:22:26.414Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":26,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"65c79256-98c2-40c8-8dae-77ad3fe5951f","EventDtm":"2025-11-25T14:22:09Z","AppDtm":"2025-11-25T14:22:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:22:09Z","DeviceID":"JSGA623040331","GPSLockState":"LOCKED","GPSSatelliteCount":14,"GPSLastLock":0,"GPSLatitude":17.516198,"GPSLongitude":82.962335,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31843","CID":"240957964","RSSI":null,"ExtPower":true,"ExtPowerVoltage":30.3,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"BMOU9782197","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:22:09Z","AssetType":"Reefer","AssetID":"BMOU9782197","OEM":"DAIKIN","TAmb":24.62,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":30,"PSucQ":"asProvided","TDis":84.3,"TDisQ":null,"FreqComp":null,"TSuc":-10.8,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":800,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":53,"PctExpVlvQ":null,"TEvap":22,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":60,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":385.3,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":24.5,"TRtn2Q":null,"TSet":23,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":10.06,"PctSucVlvQ":null,"TSup1":23.12,"TSup1Q":null,"TSup2":23.1,"TSup2Q":null,"AmpTotalDraw":11,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-09-09T22:31:45Z","PTIResult":"Unknown","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:22:27.431Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":27,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"8dc52125-c646-4c1b-818d-3d9eec839576","EventDtm":"2025-11-25T14:22:14Z","AppDtm":"2025-11-25T14:22:26Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:22:14Z","DeviceID":"JSGA622180045","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":26.310585,"GPSLongitude":91.717632,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"56","LAC":"7134","CID":"250551313","RSSI":null,"ExtPower":true,"ExtPowerVoltage":32.5,"BatteryVoltage":8,"DeviceTemp":24,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7151905","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:22:14Z","AssetType":"Reefer","AssetID":"TDRU7151905","OEM":"DAIKIN","TAmb":23,"TAmbQ":null,"TUSDA4":-46.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-20,"PSucQ":"asProvided","TDis":68.3,"TDisQ":null,"FreqComp":null,"TSuc":-28.9,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":840,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":70,"PctExpVlvQ":null,"TEvap":-0.06,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":407,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":-0.06,"TRtn1Q":null,"TRtn2":5.1,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C2","VerSWMinor":null,"PctSucVlv":84.76,"PctSucVlvQ":null,"TSup1":4.12,"TSup1Q":null,"TSup2":3.9,"TSup2Q":null,"AmpTotalDraw":10,"AmpTotalDrawQ":"asProvided","TUSDA1":-46.4,"TUSDA1Q":"OOR","TUSDA2":-46.3,"TUSDA2Q":"OOR","TUSDA3":-46.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":[{"OemAlarm":403,"RCAlias":"E403","RCSeverity":"Minor","Active":true},{"OemAlarm":409,"RCAlias":"E409","RCSeverity":"Informational","Active":true}]}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:23:53.421Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":28,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"dbb4e5b9-8c9d-4a03-a1ef-e1843da4b153","EventDtm":"2025-11-25T14:23:35Z","AppDtm":"2025-11-25T14:23:53Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:23:35Z","DeviceID":"JSGA622340343","GPSLockState":"LOCKED","GPSSatelliteCount":15,"GPSLastLock":0,"GPSLatitude":12.804949,"GPSLongitude":77.662233,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"45","LAC":"9003","CID":"46904076","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:23:35Z","AssetType":"Reefer","AssetID":"CCLU1035976","OEM":"CARRIER","TAmb":30.13,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":5,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.88,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":89.17,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04904656","AmpPhA":11.33,"AmpPhB":11.21,"AmpPhC":11.33,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":6.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":0,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.89,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":5.74,"TRtn1Q":null,"TRtn2":5.76,"TRtn2Q":null,"TSet":5,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.58,"PctSucVlvQ":null,"TSup1":5.05,"TSup1Q":null,"TSup2":5,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-05-12T10:01:32Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:24:56.915Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":29,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"36df996e-9fbb-4176-924c-0605e4e5705b","EventDtm":"2025-11-25T14:24:42Z","AppDtm":"2025-11-25T14:24:55Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:24:42Z","DeviceID":"JSGA623040313","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.364709,"GPSLongitude":75.581341,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"70","LAC":"1009","CID":"247299667","RSSI":"-79","ExtPower":true,"ExtPowerVoltage":34.1,"BatteryVoltage":8,"DeviceTemp":22,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"MORU0322200","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:24:42Z","AssetType":"Reefer","AssetID":"MORU0322200","OEM":"THERMOKING","TAmb":15,"TAmbQ":"asProvided","TUSDA4":3276.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":null,"PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":3276.6,"PSucQ":"unavailable","TDis":3276.6,"TDisQ":"OOR","FreqComp":50,"TSuc":3276.6,"TSucQ":"unavailable","MCond":null,"PCond":3276.6,"PCondQ":"unavailable","TCond":38,"TCondQ":"asProvided","MCtrl":"MaintainCool","SnCtrl":"E001083433","AmpPhA":5.3,"AmpPhB":6.2,"AmpPhC":6,"PDis":3276.6,"PDisQ":"unavailable","PctEconVlv":255,"PctEconVlvQ":"notUsed","PctExpVlv":255,"PctExpVlvQ":"notUsed","TEvap":16.9,"TEvapQ":"asProvided","MCtrl3":"Chilled","PctHtr":255,"PctHtrQ":"notUsed","MEvapFanHS":null,"PctGasVlv":255,"PctGasVlvQ":"notUsed","PctHum":255,"PctHumQ":"OOR","PctHumSet":255,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":404,"VLine2":null,"VLine3":null,"MEvapFanLS":null,"PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":null,"TRtn1":16.2,"TRtn1Q":"asProvided","TRtn2":3276.6,"TRtn2Q":"OOR","TSet":16,"TSetQ":null,"VerSWMajor":"12060800","VerSWMinor":null,"PctSucVlv":255,"PctSucVlvQ":"notUsed","TSup1":16,"TSup1Q":"asProvided","TSup2":16,"TSup2Q":"asProvided","AmpTotalDraw":7.7,"AmpTotalDrawQ":null,"TUSDA1":3276.4,"TUSDA1Q":"OOR","TUSDA2":3276.4,"TUSDA2Q":"OOR","TUSDA3":3276.4,"TUSDA3Q":"OOR","CmhVent":1275,"CmhVentQ":"OOR","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":null,"PTIResult":null,"TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
+  </si>
+  <si>
+    <t>2025-11-25T14:25:50.079Z</t>
+  </si>
+  <si>
+    <t>{"Sequence":30,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"6f7919d3-3363-4bbc-bc19-7b6f7de537b0","EventDtm":"2025-11-25T14:25:36Z","AppDtm":"2025-11-25T14:25:49Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T14:25:36Z","DeviceID":"JSGA623040285","GPSLockState":"LOCKED","GPSSatelliteCount":18,"GPSLastLock":0,"GPSLatitude":17.51617,"GPSLongitude":82.981183,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31122","CID":"239136277","RSSI":"-67","ExtPower":true,"ExtPowerVoltage":29.9,"BatteryVoltage":8,"DeviceTemp":33,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6680994","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T14:25:36Z","AssetType":"Reefer","AssetID":"TRIU6680994","OEM":"CARRIER","TAmb":27.06,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":3,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-196.48,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":137.75,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04960884","AmpPhA":11.75,"AmpPhB":10.85,"AmpPhC":11.75,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":3.45,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":96.1,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":416.6,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":0.06,"PctO2Q":"unknown","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":3.7,"TRtn1Q":null,"TRtn2":3.73,"TRtn2Q":null,"TSet":3,"TSetQ":null,"VerSWMajor":"5178","VerSWMinor":null,"PctSucVlv":4.66,"PctSucVlvQ":null,"TSup1":3.06,"TSup1Q":null,"TSup2":3.06,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2024-04-27T14:06:01Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":null}}}</t>
   </si>
 </sst>
 </file>
@@ -546,7 +612,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1205,6 +1271,358 @@
         <v>48</v>
       </c>
     </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Fix: correct technician assigned services + proper auto-assign logic
</commit_message>
<xml_diff>
--- a/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
+++ b/logs/orbcomm/orbcomm_alerts_2025-11-25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Timestamp</t>
   </si>
@@ -43,43 +43,13 @@
     <t>Raw JSON</t>
   </si>
   <si>
-    <t>2025-11-25T05:09:32.858Z</t>
+    <t>2025-11-25T19:02:41.814Z</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3069296c-1c74-4b2c-b7f5-110235cc7097","EventDtm":"2025-11-25T05:05:31Z","AppDtm":"2025-11-25T05:05:44Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:05:31Z","DeviceID":"JSGA623040295","GPSLockState":"LOCKED","GPSSatelliteCount":17,"GPSLastLock":0,"GPSLatitude":17.679062,"GPSLongitude":78.720067,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19328","CID":"254963202","RSSI":null,"ExtPower":true,"ExtPowerVoltage":29.4,"BatteryVoltage":8,"DeviceTemp":32,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CGMU2991560","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:05:31Z","AssetType":"Reefer","AssetID":"CGMU2991560","OEM":"CARRIER","TAmb":25.38,"TAmbQ":null,"TUSDA4":-50,"TUSDA4Q":"OOR","PctCO2":4,"PctCO2Q":null,"PctCO2Set":1,"PctCO2SetQ":null,"PSuc":-14.73,"PSucQ":"OOR","TDis":-182.03,"TDisQ":"OOR","FreqComp":null,"TSuc":0,"TSucQ":null,"MCond":1,"PCond":137.41,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":"Cool","SnCtrl":"04540798","AmpPhA":11.1,"AmpPhB":10.76,"AmpPhC":11.1,"PDis":-14.6,"PDisQ":"OOR","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":0,"PctExpVlvQ":null,"TEvap":5.19,"TEvapQ":null,"MCtrl3":null,"PctHtr":null,"PctHtrQ":null,"MEvapFanHS":1,"PctGasVlv":null,"PctGasVlvQ":null,"PctHum":100,"PctHumQ":null,"PctHumSet":0,"PctHumSetQ":"OOR","FreqLine":50,"FreqLineQ":null,"VLine1":411.78,"VLine2":null,"VLine3":null,"MEvapFanLS":0,"PctO2":-0.06,"PctO2Q":"OOR","PctO2Set":3,"PctO2SetQ":null,"MCtrl2":null,"TRtn1":4.71,"TRtn1Q":null,"TRtn2":4.71,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"5180","VerSWMinor":null,"PctSucVlv":3.65,"PctSucVlvQ":null,"TSup1":3.92,"TSup1Q":null,"TSup2":3.96,"TSup2Q":null,"AmpTotalDraw":null,"AmpTotalDrawQ":null,"TUSDA1":-50,"TUSDA1Q":"OOR","TUSDA2":-50,"TUSDA2Q":"OOR","TUSDA3":-50,"TUSDA3Q":"OOR","CmhVent":0,"CmhVentQ":null,"BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-09-11T07:51:42Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":null,"ReeferAlarms":[{"OemAlarm":53,"RCAlias":"AL53","RCSeverity":"Informational","Active":true}]}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:09:32.929Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":2,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"3aa492ca-003a-4aa8-a1eb-24189d6ec752","EventDtm":"2025-11-25T06:49:58Z","AppDtm":"2025-11-25T05:08:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T06:49:58Z","DeviceID":"JSGA622180057","GPSLockState":"UNLOCKED","GPSSatelliteCount":255,"GPSLastLock":3699,"GPSLatitude":17.244358,"GPSLongitude":78.443679,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"32291","CID":"244550678","RSSI":"-73","ExtPower":true,"ExtPowerVoltage":34.3,"BatteryVoltage":8.1,"DeviceTemp":30,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":null,"LastAssetRunState":null},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:09:33.467Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":3,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"726959ca-0b44-4f97-9723-125c5a379a9e","EventDtm":"2025-11-25T05:09:08Z","AppDtm":"2025-11-25T05:09:30Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:09:08Z","DeviceID":"JSGA623040290","GPSLockState":"LOCKED","GPSSatelliteCount":16,"GPSLastLock":0,"GPSLatitude":17.661547,"GPSLongitude":83.089111,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"31121","CID":"232671233","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":30,"BatteryVoltage":8,"DeviceTemp":34,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TDRU7153256","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T05:09:08Z","AssetType":"Reefer","AssetID":"TDRU7153256","OEM":"DAIKIN","TAmb":30.5,"TAmbQ":null,"TUSDA4":-72.8,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":50,"PSucQ":"asProvided","TDis":46.2,"TDisQ":null,"FreqComp":null,"TSuc":-14,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":1060,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":18,"PctExpVlvQ":null,"TEvap":3.5,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":75,"PctHumSetQ":"configured","FreqLine":50,"FreqLineQ":null,"VLine1":367.5,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":5.38,"TRtn1Q":null,"TRtn2":5.3,"TRtn2Q":null,"TSet":4,"TSetQ":null,"VerSWMajor":"24C1","VerSWMinor":null,"PctSucVlv":98.78,"PctSucVlvQ":null,"TSup1":4.19,"TSup1Q":null,"TSup2":4.1,"TSup2Q":null,"AmpTotalDraw":14,"AmpTotalDrawQ":"asProvided","TUSDA1":-72.7,"TUSDA1Q":"OOR","TUSDA2":-72.8,"TUSDA2Q":"OOR","TUSDA3":-72.8,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-04-24T05:53:24Z","PTIResult":"Passed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:10:38.675Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":4,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"aecd3425-d975-4115-960d-d7fb04ad05bf","EventDtm":"2025-11-25T05:10:22Z","AppDtm":"2025-11-25T05:10:37Z","Events":["BatteryPowerOn"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:10:22Z","DeviceID":"JSGA623040193","GPSLockState":"LOCKED","GPSSatelliteCount":13,"GPSLastLock":0,"GPSLatitude":28.678715,"GPSLongitude":77.59958,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"97","LAC":"1827","CID":"230077975","RSSI":"-67","ExtPower":false,"ExtPowerVoltage":4.7,"BatteryVoltage":7.9,"DeviceTemp":26,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"SJKU4000017","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:11:21.444Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":5,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"30770747-3acc-4083-ae91-0ed242ad587d","EventDtm":"2025-11-25T05:11:08Z","AppDtm":"2025-11-25T05:11:20Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:08Z","DeviceID":"JSGA623040302","GPSLockState":"LOCKED","GPSSatelliteCount":10,"GPSLastLock":4,"GPSLatitude":19.252921,"GPSLongitude":73.016577,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"90","LAC":"6253","CID":"249578853","RSSI":"-65","ExtPower":true,"ExtPowerVoltage":28.9,"BatteryVoltage":8,"DeviceTemp":35,"RTDLOn":false,"VerFW":"W0206 1.41","DeviceType":"CT3500","DoorState":"Open","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"TRIU6681882","LastAssetRunState":"Running"},"ReeferData":null}}</t>
-  </si>
-  <si>
-    <t>2025-11-25T05:11:28.473Z</t>
-  </si>
-  <si>
-    <t>{"Sequence":6,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"2b5837cc-f513-403f-b53a-83c0ced9ccc6","EventDtm":"2025-11-25T05:11:07Z","AppDtm":"2025-11-25T05:11:27Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T05:11:07Z","DeviceID":"JSGA623040329","GPSLockState":"UNLOCKED","GPSSatelliteCount":10,"GPSLastLock":12,"GPSLatitude":17.547937,"GPSLongitude":78.380464,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"404","MNC":"49","LAC":"19392","CID":"232207115","RSSI":"-59","ExtPower":true,"ExtPowerVoltage":32.7,"BatteryVoltage":8,"DeviceTemp":28,"RTDLOn":false,"VerFW":"W0206 1.91","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CCLU1035976","LastAssetRunState":"Offline"},"ReeferData":null}}</t>
+    <t>{"Sequence":1,"Event":{"EventClass":"DeviceMessage","MessageData":{"MsgID":"a3f6808f-a153-4ec0-901d-867e2662dacd","EventDtm":"2025-11-25T19:02:25Z","AppDtm":"2025-11-25T19:02:41Z","Events":["ScheduledReport"]},"DeviceData":{"DeviceDataDtm":"2025-11-25T19:02:25Z","DeviceID":"JSGA621320217","GPSLockState":"LOCKED","GPSSatelliteCount":20,"GPSLastLock":0,"GPSLatitude":26.644599,"GPSLongitude":88.467988,"GeofenceCode":null,"ServerGeofenceCode":null,"MCC":"405","MNC":"51","LAC":"41512","CID":"16323942","RSSI":null,"ExtPower":true,"ExtPowerVoltage":34,"BatteryVoltage":8.1,"DeviceTemp":25,"RTDLOn":false,"VerFW":"W0206 1.75","DeviceType":"CT3500","DoorState":"Disconnected","DoorStateDtm":null,"DoorSensorBatteryVoltage":null,"LastAssetID":"CXRU1036301","LastAssetRunState":"Running"},"ReeferData":{"ReeferDataDtm":"2025-11-25T19:02:25Z","AssetType":"Reefer","AssetID":"CXRU1036301","OEM":"DAIKIN","TAmb":18.81,"TAmbQ":null,"TUSDA4":-53.4,"TUSDA4Q":"OOR","PctCO2":25.5,"PctCO2Q":"OOR","PctCO2Set":25.5,"PctCO2SetQ":"OOR","PSuc":-10,"PSucQ":"asProvided","TDis":64.3,"TDisQ":null,"FreqComp":null,"TSuc":-24.3,"TSucQ":null,"MCond":"On","PCond":null,"PCondQ":null,"TCond":null,"TCondQ":null,"MCtrl":null,"SnCtrl":null,"AmpPhA":null,"AmpPhB":null,"AmpPhC":null,"PDis":830,"PDisQ":"asProvided","PctEconVlv":0,"PctEconVlvQ":null,"PctExpVlv":25,"PctExpVlvQ":null,"TEvap":-1.38,"TEvapQ":null,"MCtrl3":"Modulation","PctHtr":null,"PctHtrQ":null,"MEvapFanHS":"On","PctGasVlv":0,"PctGasVlvQ":null,"PctHum":100.39,"PctHumQ":"OOR","PctHumSet":65,"PctHumSetQ":"off","FreqLine":null,"FreqLineQ":null,"VLine1":424.8,"VLine2":null,"VLine3":null,"MEvapFanLS":"Off","PctO2":25.5,"PctO2Q":"OOR","PctO2Set":25.5,"PctO2SetQ":"OOR","MCtrl2":"Modulation","TRtn1":1.19,"TRtn1Q":null,"TRtn2":1.9,"TRtn2Q":null,"TSet":0,"TSetQ":null,"VerSWMajor":"265A","VerSWMinor":null,"PctSucVlv":12.8,"PctSucVlvQ":null,"TSup1":0.19,"TSup1Q":null,"TSup2":1.8,"TSup2Q":null,"AmpTotalDraw":13,"AmpTotalDrawQ":"asProvided","TUSDA1":-53.4,"TUSDA1Q":"OOR","TUSDA2":-53.4,"TUSDA2Q":"OOR","TUSDA3":-53.4,"TUSDA3Q":"OOR","CmhVent":1020,"CmhVentQ":"error","BkNum":null,"TBk":null,"TBkQ":null,"PTIDtm":"2025-07-16T10:29:07Z","PTIResult":"Failed","TWResult":null,"TWExpiration":null,"TWExpirationQ":null,"AtmosMode":"UnitOff","ReeferAlarms":null}}}</t>
   </si>
 </sst>
 </file>
@@ -468,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -551,166 +521,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>